<commit_message>
Some load list changes completed
</commit_message>
<xml_diff>
--- a/thermax_backend/templates/enviro_load_list_template.xlsx
+++ b/thermax_backend/templates/enviro_load_list_template.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\abhishekraje30\frappe-bench\apps\thermax_backend\thermax_backend\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76BAEF4D-6C5D-486E-8E90-143A8DCD3921}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C0A61D7-574B-40A8-9399-9E5C2F69A0F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="678" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="678" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="COVER" sheetId="9" r:id="rId1"/>
-    <sheet name="NOTES " sheetId="10" r:id="rId2"/>
+    <sheet name="NOTES" sheetId="10" r:id="rId2"/>
     <sheet name="LOAD LIST OUTPUT" sheetId="8" r:id="rId3"/>
   </sheets>
   <externalReferences>
@@ -26,7 +26,7 @@
     <definedName name="CABLEOD">#REF!</definedName>
     <definedName name="DATA1">[1]Sheet1!$C$5:$J$25</definedName>
     <definedName name="pf">'[2]Cable cal'!#REF!</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="1">'NOTES '!$A$1:$Q$23</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">NOTES!$A$1:$Q$23</definedName>
     <definedName name="RANGE1">[3]PGD!#REF!</definedName>
     <definedName name="Vd">(3)^0.5*'[2]Cable cal'!XET1*('[2]Cable cal'!XFB1*0.8+'[2]Cable cal'!XFC1*0.6)*'[2]Cable cal'!XFD1/1000</definedName>
     <definedName name="Vd_R">(3)^0.5*'[2]Cable cal'!XES1*('[2]Cable cal'!XFB1*'[2]Cable cal'!XEQ1+'[2]Cable cal'!XFC1*((1-'[2]Cable cal'!#REF!^2)^0.5))*'[2]Cable cal'!XFD1/1000</definedName>
@@ -1383,6 +1383,57 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="32" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="33" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="34" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="12" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="14" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="35" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="36" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="37" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="36" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="38" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
@@ -1419,56 +1470,41 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="40" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="32" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="33" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="34" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="11" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="12" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="14" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="35" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="36" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="37" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="36" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="38" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="18" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1476,6 +1512,18 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1485,53 +1533,44 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="14" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="11" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="18" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1549,45 +1588,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2280,7 +2280,7 @@
   </sheetPr>
   <dimension ref="A1:CD35"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A2" zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="70" workbookViewId="0">
+    <sheetView view="pageBreakPreview" topLeftCell="A2" zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="70" workbookViewId="0">
       <selection activeCell="D10" sqref="D10:G10"/>
     </sheetView>
   </sheetViews>
@@ -2929,50 +2929,50 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="116.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="51"/>
-      <c r="B1" s="52"/>
-      <c r="C1" s="52"/>
-      <c r="D1" s="52"/>
-      <c r="E1" s="52"/>
-      <c r="F1" s="52"/>
-      <c r="G1" s="52"/>
-      <c r="H1" s="53"/>
+      <c r="A1" s="39"/>
+      <c r="B1" s="40"/>
+      <c r="C1" s="40"/>
+      <c r="D1" s="40"/>
+      <c r="E1" s="40"/>
+      <c r="F1" s="40"/>
+      <c r="G1" s="40"/>
+      <c r="H1" s="41"/>
     </row>
     <row r="2" spans="1:8" ht="26.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="54" t="s">
+      <c r="A2" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="55"/>
-      <c r="C2" s="55"/>
-      <c r="D2" s="55"/>
-      <c r="E2" s="55"/>
-      <c r="F2" s="55"/>
-      <c r="G2" s="55"/>
-      <c r="H2" s="56"/>
+      <c r="B2" s="43"/>
+      <c r="C2" s="43"/>
+      <c r="D2" s="43"/>
+      <c r="E2" s="43"/>
+      <c r="F2" s="43"/>
+      <c r="G2" s="43"/>
+      <c r="H2" s="44"/>
     </row>
     <row r="3" spans="1:8" ht="23.5" x14ac:dyDescent="0.3">
-      <c r="A3" s="57" t="s">
+      <c r="A3" s="45" t="s">
         <v>74</v>
       </c>
-      <c r="B3" s="58"/>
-      <c r="C3" s="58"/>
-      <c r="D3" s="58"/>
-      <c r="E3" s="58"/>
-      <c r="F3" s="58"/>
-      <c r="G3" s="58"/>
-      <c r="H3" s="59"/>
+      <c r="B3" s="46"/>
+      <c r="C3" s="46"/>
+      <c r="D3" s="46"/>
+      <c r="E3" s="46"/>
+      <c r="F3" s="46"/>
+      <c r="G3" s="46"/>
+      <c r="H3" s="47"/>
     </row>
     <row r="4" spans="1:8" ht="24" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="60" t="s">
+      <c r="A4" s="48" t="s">
         <v>73</v>
       </c>
-      <c r="B4" s="61"/>
-      <c r="C4" s="61"/>
-      <c r="D4" s="61"/>
-      <c r="E4" s="61"/>
-      <c r="F4" s="61"/>
-      <c r="G4" s="61"/>
-      <c r="H4" s="62"/>
+      <c r="B4" s="49"/>
+      <c r="C4" s="49"/>
+      <c r="D4" s="49"/>
+      <c r="E4" s="49"/>
+      <c r="F4" s="49"/>
+      <c r="G4" s="49"/>
+      <c r="H4" s="50"/>
     </row>
     <row r="5" spans="1:8" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="4"/>
@@ -2986,76 +2986,76 @@
     </row>
     <row r="6" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4"/>
-      <c r="B6" s="63" t="s">
+      <c r="B6" s="51" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="64"/>
-      <c r="D6" s="65" t="s">
+      <c r="C6" s="52"/>
+      <c r="D6" s="53" t="s">
         <v>2</v>
       </c>
-      <c r="E6" s="66"/>
-      <c r="F6" s="66"/>
-      <c r="G6" s="67"/>
+      <c r="E6" s="54"/>
+      <c r="F6" s="54"/>
+      <c r="G6" s="55"/>
       <c r="H6" s="6"/>
     </row>
     <row r="7" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="4"/>
-      <c r="B7" s="49" t="s">
+      <c r="B7" s="66" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="50"/>
-      <c r="D7" s="41"/>
-      <c r="E7" s="42"/>
-      <c r="F7" s="42"/>
-      <c r="G7" s="43"/>
+      <c r="C7" s="67"/>
+      <c r="D7" s="58"/>
+      <c r="E7" s="59"/>
+      <c r="F7" s="59"/>
+      <c r="G7" s="60"/>
       <c r="H7" s="6"/>
     </row>
     <row r="8" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4"/>
-      <c r="B8" s="39" t="s">
+      <c r="B8" s="56" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="40"/>
-      <c r="D8" s="41"/>
-      <c r="E8" s="42"/>
-      <c r="F8" s="42"/>
-      <c r="G8" s="43"/>
+      <c r="C8" s="57"/>
+      <c r="D8" s="58"/>
+      <c r="E8" s="59"/>
+      <c r="F8" s="59"/>
+      <c r="G8" s="60"/>
       <c r="H8" s="6"/>
     </row>
     <row r="9" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="4"/>
-      <c r="B9" s="39" t="s">
+      <c r="B9" s="56" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="40"/>
-      <c r="D9" s="41"/>
-      <c r="E9" s="42"/>
-      <c r="F9" s="42"/>
-      <c r="G9" s="43"/>
+      <c r="C9" s="57"/>
+      <c r="D9" s="58"/>
+      <c r="E9" s="59"/>
+      <c r="F9" s="59"/>
+      <c r="G9" s="60"/>
       <c r="H9" s="6"/>
     </row>
     <row r="10" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="4"/>
-      <c r="B10" s="39" t="s">
+      <c r="B10" s="56" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="40"/>
-      <c r="D10" s="41"/>
-      <c r="E10" s="42"/>
-      <c r="F10" s="42"/>
-      <c r="G10" s="43"/>
+      <c r="C10" s="57"/>
+      <c r="D10" s="58"/>
+      <c r="E10" s="59"/>
+      <c r="F10" s="59"/>
+      <c r="G10" s="60"/>
       <c r="H10" s="6"/>
     </row>
     <row r="11" spans="1:8" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="4"/>
-      <c r="B11" s="44" t="s">
+      <c r="B11" s="61" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="45"/>
-      <c r="D11" s="46"/>
-      <c r="E11" s="47"/>
-      <c r="F11" s="47"/>
-      <c r="G11" s="48"/>
+      <c r="C11" s="62"/>
+      <c r="D11" s="63"/>
+      <c r="E11" s="64"/>
+      <c r="F11" s="64"/>
+      <c r="G11" s="65"/>
       <c r="H11" s="6"/>
     </row>
     <row r="12" spans="1:8" s="9" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -3319,12 +3319,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="A2:H2"/>
-    <mergeCell ref="A3:H3"/>
-    <mergeCell ref="A4:H4"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="D6:G6"/>
     <mergeCell ref="B10:C10"/>
     <mergeCell ref="D10:G10"/>
     <mergeCell ref="B11:C11"/>
@@ -3335,6 +3329,12 @@
     <mergeCell ref="D8:G8"/>
     <mergeCell ref="B9:C9"/>
     <mergeCell ref="D9:G9"/>
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A2:H2"/>
+    <mergeCell ref="A3:H3"/>
+    <mergeCell ref="A4:H4"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="D6:G6"/>
   </mergeCells>
   <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="66" fitToHeight="100" orientation="portrait" r:id="rId1"/>
@@ -3346,7 +3346,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Q23"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" zoomScale="90" zoomScaleNormal="100" zoomScaleSheetLayoutView="90" workbookViewId="0">
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="90" zoomScaleNormal="100" zoomScaleSheetLayoutView="90" workbookViewId="0">
       <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
@@ -3358,533 +3358,534 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="70" t="s">
+      <c r="A1" s="86" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="71"/>
-      <c r="C1" s="71"/>
-      <c r="D1" s="71"/>
-      <c r="E1" s="71"/>
-      <c r="F1" s="71"/>
-      <c r="G1" s="71"/>
-      <c r="H1" s="71"/>
-      <c r="I1" s="71"/>
-      <c r="J1" s="71"/>
-      <c r="K1" s="71"/>
-      <c r="L1" s="71"/>
-      <c r="M1" s="71"/>
-      <c r="N1" s="71"/>
-      <c r="O1" s="71"/>
-      <c r="P1" s="71"/>
-      <c r="Q1" s="72"/>
+      <c r="B1" s="87"/>
+      <c r="C1" s="87"/>
+      <c r="D1" s="87"/>
+      <c r="E1" s="87"/>
+      <c r="F1" s="87"/>
+      <c r="G1" s="87"/>
+      <c r="H1" s="87"/>
+      <c r="I1" s="87"/>
+      <c r="J1" s="87"/>
+      <c r="K1" s="87"/>
+      <c r="L1" s="87"/>
+      <c r="M1" s="87"/>
+      <c r="N1" s="87"/>
+      <c r="O1" s="87"/>
+      <c r="P1" s="87"/>
+      <c r="Q1" s="88"/>
     </row>
     <row r="2" spans="1:17" ht="13" x14ac:dyDescent="0.25">
       <c r="A2" s="34" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="73" t="s">
+      <c r="B2" s="84" t="s">
         <v>81</v>
       </c>
-      <c r="C2" s="73"/>
-      <c r="D2" s="73"/>
-      <c r="E2" s="73"/>
-      <c r="F2" s="73"/>
-      <c r="G2" s="73"/>
-      <c r="H2" s="73"/>
-      <c r="I2" s="73"/>
-      <c r="J2" s="73"/>
-      <c r="K2" s="73"/>
-      <c r="L2" s="73"/>
-      <c r="M2" s="73"/>
-      <c r="N2" s="73"/>
-      <c r="O2" s="73"/>
-      <c r="P2" s="73"/>
-      <c r="Q2" s="74"/>
+      <c r="C2" s="84"/>
+      <c r="D2" s="84"/>
+      <c r="E2" s="84"/>
+      <c r="F2" s="84"/>
+      <c r="G2" s="84"/>
+      <c r="H2" s="84"/>
+      <c r="I2" s="84"/>
+      <c r="J2" s="84"/>
+      <c r="K2" s="84"/>
+      <c r="L2" s="84"/>
+      <c r="M2" s="84"/>
+      <c r="N2" s="84"/>
+      <c r="O2" s="84"/>
+      <c r="P2" s="84"/>
+      <c r="Q2" s="85"/>
     </row>
     <row r="3" spans="1:17" ht="13" x14ac:dyDescent="0.25">
       <c r="A3" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="73" t="s">
+      <c r="B3" s="84" t="s">
         <v>82</v>
       </c>
-      <c r="C3" s="73"/>
-      <c r="D3" s="73"/>
-      <c r="E3" s="73"/>
-      <c r="F3" s="73"/>
-      <c r="G3" s="73"/>
-      <c r="H3" s="73"/>
-      <c r="I3" s="73"/>
-      <c r="J3" s="73"/>
-      <c r="K3" s="73"/>
-      <c r="L3" s="73"/>
-      <c r="M3" s="73"/>
-      <c r="N3" s="73"/>
-      <c r="O3" s="73"/>
-      <c r="P3" s="73"/>
-      <c r="Q3" s="74"/>
+      <c r="C3" s="84"/>
+      <c r="D3" s="84"/>
+      <c r="E3" s="84"/>
+      <c r="F3" s="84"/>
+      <c r="G3" s="84"/>
+      <c r="H3" s="84"/>
+      <c r="I3" s="84"/>
+      <c r="J3" s="84"/>
+      <c r="K3" s="84"/>
+      <c r="L3" s="84"/>
+      <c r="M3" s="84"/>
+      <c r="N3" s="84"/>
+      <c r="O3" s="84"/>
+      <c r="P3" s="84"/>
+      <c r="Q3" s="85"/>
     </row>
     <row r="4" spans="1:17" ht="13" x14ac:dyDescent="0.25">
       <c r="A4" s="34" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="73" t="s">
+      <c r="B4" s="84" t="s">
         <v>83</v>
       </c>
-      <c r="C4" s="73"/>
-      <c r="D4" s="73"/>
-      <c r="E4" s="73"/>
-      <c r="F4" s="73"/>
-      <c r="G4" s="73"/>
-      <c r="H4" s="73"/>
-      <c r="I4" s="73"/>
-      <c r="J4" s="73"/>
-      <c r="K4" s="73"/>
-      <c r="L4" s="73"/>
-      <c r="M4" s="73"/>
-      <c r="N4" s="73"/>
-      <c r="O4" s="73"/>
-      <c r="P4" s="73"/>
-      <c r="Q4" s="74"/>
+      <c r="C4" s="84"/>
+      <c r="D4" s="84"/>
+      <c r="E4" s="84"/>
+      <c r="F4" s="84"/>
+      <c r="G4" s="84"/>
+      <c r="H4" s="84"/>
+      <c r="I4" s="84"/>
+      <c r="J4" s="84"/>
+      <c r="K4" s="84"/>
+      <c r="L4" s="84"/>
+      <c r="M4" s="84"/>
+      <c r="N4" s="84"/>
+      <c r="O4" s="84"/>
+      <c r="P4" s="84"/>
+      <c r="Q4" s="85"/>
     </row>
     <row r="5" spans="1:17" ht="13" x14ac:dyDescent="0.25">
       <c r="A5" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="73" t="s">
+      <c r="B5" s="84" t="s">
         <v>84</v>
       </c>
-      <c r="C5" s="73"/>
-      <c r="D5" s="73"/>
-      <c r="E5" s="73"/>
-      <c r="F5" s="73"/>
-      <c r="G5" s="73"/>
-      <c r="H5" s="73"/>
-      <c r="I5" s="73"/>
-      <c r="J5" s="73"/>
-      <c r="K5" s="73"/>
-      <c r="L5" s="73"/>
-      <c r="M5" s="73"/>
-      <c r="N5" s="73"/>
-      <c r="O5" s="73"/>
-      <c r="P5" s="73"/>
-      <c r="Q5" s="74"/>
+      <c r="C5" s="84"/>
+      <c r="D5" s="84"/>
+      <c r="E5" s="84"/>
+      <c r="F5" s="84"/>
+      <c r="G5" s="84"/>
+      <c r="H5" s="84"/>
+      <c r="I5" s="84"/>
+      <c r="J5" s="84"/>
+      <c r="K5" s="84"/>
+      <c r="L5" s="84"/>
+      <c r="M5" s="84"/>
+      <c r="N5" s="84"/>
+      <c r="O5" s="84"/>
+      <c r="P5" s="84"/>
+      <c r="Q5" s="85"/>
     </row>
     <row r="6" spans="1:17" ht="13" x14ac:dyDescent="0.25">
       <c r="A6" s="34" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="68" t="s">
+      <c r="B6" s="80" t="s">
         <v>85</v>
       </c>
-      <c r="C6" s="68"/>
-      <c r="D6" s="68"/>
-      <c r="E6" s="68"/>
-      <c r="F6" s="68"/>
-      <c r="G6" s="68"/>
-      <c r="H6" s="68"/>
-      <c r="I6" s="68"/>
-      <c r="J6" s="68"/>
-      <c r="K6" s="68"/>
-      <c r="L6" s="68"/>
-      <c r="M6" s="68"/>
-      <c r="N6" s="68"/>
-      <c r="O6" s="68"/>
-      <c r="P6" s="68"/>
-      <c r="Q6" s="69"/>
+      <c r="C6" s="80"/>
+      <c r="D6" s="80"/>
+      <c r="E6" s="80"/>
+      <c r="F6" s="80"/>
+      <c r="G6" s="80"/>
+      <c r="H6" s="80"/>
+      <c r="I6" s="80"/>
+      <c r="J6" s="80"/>
+      <c r="K6" s="80"/>
+      <c r="L6" s="80"/>
+      <c r="M6" s="80"/>
+      <c r="N6" s="80"/>
+      <c r="O6" s="80"/>
+      <c r="P6" s="80"/>
+      <c r="Q6" s="81"/>
     </row>
     <row r="7" spans="1:17" ht="13" x14ac:dyDescent="0.25">
       <c r="A7" s="34" t="s">
         <v>21</v>
       </c>
-      <c r="B7" s="68" t="s">
+      <c r="B7" s="80" t="s">
         <v>86</v>
       </c>
-      <c r="C7" s="68"/>
-      <c r="D7" s="68"/>
-      <c r="E7" s="68"/>
-      <c r="F7" s="68"/>
-      <c r="G7" s="68"/>
-      <c r="H7" s="68"/>
-      <c r="I7" s="68"/>
-      <c r="J7" s="68"/>
-      <c r="K7" s="68"/>
-      <c r="L7" s="68"/>
-      <c r="M7" s="68"/>
-      <c r="N7" s="68"/>
-      <c r="O7" s="68"/>
-      <c r="P7" s="68"/>
-      <c r="Q7" s="69"/>
+      <c r="C7" s="80"/>
+      <c r="D7" s="80"/>
+      <c r="E7" s="80"/>
+      <c r="F7" s="80"/>
+      <c r="G7" s="80"/>
+      <c r="H7" s="80"/>
+      <c r="I7" s="80"/>
+      <c r="J7" s="80"/>
+      <c r="K7" s="80"/>
+      <c r="L7" s="80"/>
+      <c r="M7" s="80"/>
+      <c r="N7" s="80"/>
+      <c r="O7" s="80"/>
+      <c r="P7" s="80"/>
+      <c r="Q7" s="81"/>
     </row>
     <row r="8" spans="1:17" ht="13" x14ac:dyDescent="0.25">
       <c r="A8" s="34" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="68" t="s">
+      <c r="B8" s="80" t="s">
         <v>87</v>
       </c>
-      <c r="C8" s="68"/>
-      <c r="D8" s="68"/>
-      <c r="E8" s="68"/>
-      <c r="F8" s="68"/>
-      <c r="G8" s="68"/>
-      <c r="H8" s="68"/>
-      <c r="I8" s="68"/>
-      <c r="J8" s="68"/>
-      <c r="K8" s="68"/>
-      <c r="L8" s="68"/>
-      <c r="M8" s="68"/>
-      <c r="N8" s="68"/>
-      <c r="O8" s="68"/>
-      <c r="P8" s="68"/>
-      <c r="Q8" s="69"/>
+      <c r="C8" s="80"/>
+      <c r="D8" s="80"/>
+      <c r="E8" s="80"/>
+      <c r="F8" s="80"/>
+      <c r="G8" s="80"/>
+      <c r="H8" s="80"/>
+      <c r="I8" s="80"/>
+      <c r="J8" s="80"/>
+      <c r="K8" s="80"/>
+      <c r="L8" s="80"/>
+      <c r="M8" s="80"/>
+      <c r="N8" s="80"/>
+      <c r="O8" s="80"/>
+      <c r="P8" s="80"/>
+      <c r="Q8" s="81"/>
     </row>
     <row r="9" spans="1:17" ht="13" x14ac:dyDescent="0.25">
       <c r="A9" s="34" t="s">
         <v>23</v>
       </c>
-      <c r="B9" s="68" t="s">
+      <c r="B9" s="80" t="s">
         <v>88</v>
       </c>
-      <c r="C9" s="68"/>
-      <c r="D9" s="68"/>
-      <c r="E9" s="68"/>
-      <c r="F9" s="68"/>
-      <c r="G9" s="68"/>
-      <c r="H9" s="68"/>
-      <c r="I9" s="68"/>
-      <c r="J9" s="68"/>
-      <c r="K9" s="68"/>
-      <c r="L9" s="68"/>
-      <c r="M9" s="68"/>
-      <c r="N9" s="68"/>
-      <c r="O9" s="68"/>
-      <c r="P9" s="68"/>
-      <c r="Q9" s="69"/>
+      <c r="C9" s="80"/>
+      <c r="D9" s="80"/>
+      <c r="E9" s="80"/>
+      <c r="F9" s="80"/>
+      <c r="G9" s="80"/>
+      <c r="H9" s="80"/>
+      <c r="I9" s="80"/>
+      <c r="J9" s="80"/>
+      <c r="K9" s="80"/>
+      <c r="L9" s="80"/>
+      <c r="M9" s="80"/>
+      <c r="N9" s="80"/>
+      <c r="O9" s="80"/>
+      <c r="P9" s="80"/>
+      <c r="Q9" s="81"/>
     </row>
     <row r="10" spans="1:17" ht="13" x14ac:dyDescent="0.25">
       <c r="A10" s="34" t="s">
         <v>24</v>
       </c>
-      <c r="B10" s="68" t="s">
+      <c r="B10" s="80" t="s">
         <v>89</v>
       </c>
-      <c r="C10" s="68"/>
-      <c r="D10" s="68"/>
-      <c r="E10" s="68"/>
-      <c r="F10" s="68"/>
-      <c r="G10" s="68"/>
-      <c r="H10" s="68"/>
-      <c r="I10" s="68"/>
-      <c r="J10" s="68"/>
-      <c r="K10" s="68"/>
-      <c r="L10" s="68"/>
-      <c r="M10" s="68"/>
-      <c r="N10" s="68"/>
-      <c r="O10" s="68"/>
-      <c r="P10" s="68"/>
-      <c r="Q10" s="69"/>
+      <c r="C10" s="80"/>
+      <c r="D10" s="80"/>
+      <c r="E10" s="80"/>
+      <c r="F10" s="80"/>
+      <c r="G10" s="80"/>
+      <c r="H10" s="80"/>
+      <c r="I10" s="80"/>
+      <c r="J10" s="80"/>
+      <c r="K10" s="80"/>
+      <c r="L10" s="80"/>
+      <c r="M10" s="80"/>
+      <c r="N10" s="80"/>
+      <c r="O10" s="80"/>
+      <c r="P10" s="80"/>
+      <c r="Q10" s="81"/>
     </row>
     <row r="11" spans="1:17" ht="13" x14ac:dyDescent="0.25">
       <c r="A11" s="34" t="s">
         <v>25</v>
       </c>
-      <c r="B11" s="68" t="s">
+      <c r="B11" s="80" t="s">
         <v>90</v>
       </c>
-      <c r="C11" s="68"/>
-      <c r="D11" s="68"/>
-      <c r="E11" s="68"/>
-      <c r="F11" s="68"/>
-      <c r="G11" s="68"/>
-      <c r="H11" s="68"/>
-      <c r="I11" s="68"/>
-      <c r="J11" s="68"/>
-      <c r="K11" s="68"/>
-      <c r="L11" s="68"/>
-      <c r="M11" s="68"/>
-      <c r="N11" s="68"/>
-      <c r="O11" s="68"/>
-      <c r="P11" s="68"/>
-      <c r="Q11" s="69"/>
+      <c r="C11" s="80"/>
+      <c r="D11" s="80"/>
+      <c r="E11" s="80"/>
+      <c r="F11" s="80"/>
+      <c r="G11" s="80"/>
+      <c r="H11" s="80"/>
+      <c r="I11" s="80"/>
+      <c r="J11" s="80"/>
+      <c r="K11" s="80"/>
+      <c r="L11" s="80"/>
+      <c r="M11" s="80"/>
+      <c r="N11" s="80"/>
+      <c r="O11" s="80"/>
+      <c r="P11" s="80"/>
+      <c r="Q11" s="81"/>
     </row>
     <row r="12" spans="1:17" ht="13" x14ac:dyDescent="0.25">
       <c r="A12" s="34" t="s">
         <v>26</v>
       </c>
-      <c r="B12" s="68" t="s">
+      <c r="B12" s="80" t="s">
         <v>91</v>
       </c>
-      <c r="C12" s="68"/>
-      <c r="D12" s="68"/>
-      <c r="E12" s="68"/>
-      <c r="F12" s="68"/>
-      <c r="G12" s="68"/>
-      <c r="H12" s="68"/>
-      <c r="I12" s="68"/>
-      <c r="J12" s="68"/>
-      <c r="K12" s="68"/>
-      <c r="L12" s="68"/>
-      <c r="M12" s="68"/>
-      <c r="N12" s="68"/>
-      <c r="O12" s="68"/>
-      <c r="P12" s="68"/>
-      <c r="Q12" s="69"/>
+      <c r="C12" s="80"/>
+      <c r="D12" s="80"/>
+      <c r="E12" s="80"/>
+      <c r="F12" s="80"/>
+      <c r="G12" s="80"/>
+      <c r="H12" s="80"/>
+      <c r="I12" s="80"/>
+      <c r="J12" s="80"/>
+      <c r="K12" s="80"/>
+      <c r="L12" s="80"/>
+      <c r="M12" s="80"/>
+      <c r="N12" s="80"/>
+      <c r="O12" s="80"/>
+      <c r="P12" s="80"/>
+      <c r="Q12" s="81"/>
     </row>
     <row r="13" spans="1:17" ht="13" x14ac:dyDescent="0.25">
       <c r="A13" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="68" t="s">
+      <c r="B13" s="80" t="s">
         <v>92</v>
       </c>
-      <c r="C13" s="68"/>
-      <c r="D13" s="68"/>
-      <c r="E13" s="68"/>
-      <c r="F13" s="68"/>
-      <c r="G13" s="68"/>
-      <c r="H13" s="68"/>
-      <c r="I13" s="68"/>
-      <c r="J13" s="68"/>
-      <c r="K13" s="68"/>
-      <c r="L13" s="68"/>
-      <c r="M13" s="68"/>
-      <c r="N13" s="68"/>
-      <c r="O13" s="68"/>
-      <c r="P13" s="68"/>
-      <c r="Q13" s="69"/>
+      <c r="C13" s="80"/>
+      <c r="D13" s="80"/>
+      <c r="E13" s="80"/>
+      <c r="F13" s="80"/>
+      <c r="G13" s="80"/>
+      <c r="H13" s="80"/>
+      <c r="I13" s="80"/>
+      <c r="J13" s="80"/>
+      <c r="K13" s="80"/>
+      <c r="L13" s="80"/>
+      <c r="M13" s="80"/>
+      <c r="N13" s="80"/>
+      <c r="O13" s="80"/>
+      <c r="P13" s="80"/>
+      <c r="Q13" s="81"/>
     </row>
     <row r="14" spans="1:17" ht="13" x14ac:dyDescent="0.25">
       <c r="A14" s="35" t="s">
         <v>27</v>
       </c>
-      <c r="B14" s="77" t="s">
+      <c r="B14" s="82" t="s">
         <v>93</v>
       </c>
-      <c r="C14" s="77"/>
-      <c r="D14" s="77"/>
-      <c r="E14" s="77"/>
-      <c r="F14" s="77"/>
-      <c r="G14" s="77"/>
-      <c r="H14" s="77"/>
-      <c r="I14" s="77"/>
-      <c r="J14" s="77"/>
-      <c r="K14" s="77"/>
-      <c r="L14" s="77"/>
-      <c r="M14" s="77"/>
-      <c r="N14" s="77"/>
-      <c r="O14" s="77"/>
-      <c r="P14" s="77"/>
-      <c r="Q14" s="78"/>
+      <c r="C14" s="82"/>
+      <c r="D14" s="82"/>
+      <c r="E14" s="82"/>
+      <c r="F14" s="82"/>
+      <c r="G14" s="82"/>
+      <c r="H14" s="82"/>
+      <c r="I14" s="82"/>
+      <c r="J14" s="82"/>
+      <c r="K14" s="82"/>
+      <c r="L14" s="82"/>
+      <c r="M14" s="82"/>
+      <c r="N14" s="82"/>
+      <c r="O14" s="82"/>
+      <c r="P14" s="82"/>
+      <c r="Q14" s="83"/>
     </row>
     <row r="15" spans="1:17" ht="13" x14ac:dyDescent="0.25">
       <c r="A15" s="34" t="s">
         <v>28</v>
       </c>
-      <c r="B15" s="73" t="s">
+      <c r="B15" s="84" t="s">
         <v>94</v>
       </c>
-      <c r="C15" s="73"/>
-      <c r="D15" s="73"/>
-      <c r="E15" s="73"/>
-      <c r="F15" s="73"/>
-      <c r="G15" s="73"/>
-      <c r="H15" s="73"/>
-      <c r="I15" s="73"/>
-      <c r="J15" s="73"/>
-      <c r="K15" s="73"/>
-      <c r="L15" s="73"/>
-      <c r="M15" s="73"/>
-      <c r="N15" s="73"/>
-      <c r="O15" s="73"/>
-      <c r="P15" s="73"/>
-      <c r="Q15" s="74"/>
+      <c r="C15" s="84"/>
+      <c r="D15" s="84"/>
+      <c r="E15" s="84"/>
+      <c r="F15" s="84"/>
+      <c r="G15" s="84"/>
+      <c r="H15" s="84"/>
+      <c r="I15" s="84"/>
+      <c r="J15" s="84"/>
+      <c r="K15" s="84"/>
+      <c r="L15" s="84"/>
+      <c r="M15" s="84"/>
+      <c r="N15" s="84"/>
+      <c r="O15" s="84"/>
+      <c r="P15" s="84"/>
+      <c r="Q15" s="85"/>
     </row>
     <row r="16" spans="1:17" ht="13" x14ac:dyDescent="0.25">
       <c r="A16" s="34" t="s">
         <v>29</v>
       </c>
-      <c r="B16" s="73" t="s">
+      <c r="B16" s="84" t="s">
         <v>95</v>
       </c>
-      <c r="C16" s="73"/>
-      <c r="D16" s="73"/>
-      <c r="E16" s="73"/>
-      <c r="F16" s="73"/>
-      <c r="G16" s="73"/>
-      <c r="H16" s="73"/>
-      <c r="I16" s="73"/>
-      <c r="J16" s="73"/>
-      <c r="K16" s="73"/>
-      <c r="L16" s="73"/>
-      <c r="M16" s="73"/>
-      <c r="N16" s="73"/>
-      <c r="O16" s="73"/>
-      <c r="P16" s="73"/>
-      <c r="Q16" s="74"/>
+      <c r="C16" s="84"/>
+      <c r="D16" s="84"/>
+      <c r="E16" s="84"/>
+      <c r="F16" s="84"/>
+      <c r="G16" s="84"/>
+      <c r="H16" s="84"/>
+      <c r="I16" s="84"/>
+      <c r="J16" s="84"/>
+      <c r="K16" s="84"/>
+      <c r="L16" s="84"/>
+      <c r="M16" s="84"/>
+      <c r="N16" s="84"/>
+      <c r="O16" s="84"/>
+      <c r="P16" s="84"/>
+      <c r="Q16" s="85"/>
     </row>
     <row r="17" spans="1:17" ht="13" x14ac:dyDescent="0.25">
       <c r="A17" s="34" t="s">
         <v>30</v>
       </c>
-      <c r="B17" s="73" t="s">
+      <c r="B17" s="84" t="s">
         <v>96</v>
       </c>
-      <c r="C17" s="73"/>
-      <c r="D17" s="73"/>
-      <c r="E17" s="73"/>
-      <c r="F17" s="73"/>
-      <c r="G17" s="73"/>
-      <c r="H17" s="73"/>
-      <c r="I17" s="73"/>
-      <c r="J17" s="73"/>
-      <c r="K17" s="73"/>
-      <c r="L17" s="73"/>
-      <c r="M17" s="73"/>
-      <c r="N17" s="73"/>
-      <c r="O17" s="73"/>
-      <c r="P17" s="73"/>
-      <c r="Q17" s="74"/>
+      <c r="C17" s="84"/>
+      <c r="D17" s="84"/>
+      <c r="E17" s="84"/>
+      <c r="F17" s="84"/>
+      <c r="G17" s="84"/>
+      <c r="H17" s="84"/>
+      <c r="I17" s="84"/>
+      <c r="J17" s="84"/>
+      <c r="K17" s="84"/>
+      <c r="L17" s="84"/>
+      <c r="M17" s="84"/>
+      <c r="N17" s="84"/>
+      <c r="O17" s="84"/>
+      <c r="P17" s="84"/>
+      <c r="Q17" s="85"/>
     </row>
     <row r="18" spans="1:17" ht="13" x14ac:dyDescent="0.25">
       <c r="A18" s="34"/>
-      <c r="B18" s="75"/>
-      <c r="C18" s="75"/>
-      <c r="D18" s="75"/>
-      <c r="E18" s="75"/>
-      <c r="F18" s="75"/>
-      <c r="G18" s="75"/>
-      <c r="H18" s="75"/>
-      <c r="I18" s="75"/>
-      <c r="J18" s="75"/>
-      <c r="K18" s="75"/>
-      <c r="L18" s="75"/>
-      <c r="M18" s="75"/>
-      <c r="N18" s="75"/>
-      <c r="O18" s="75"/>
-      <c r="P18" s="75"/>
-      <c r="Q18" s="76"/>
+      <c r="B18" s="78"/>
+      <c r="C18" s="78"/>
+      <c r="D18" s="78"/>
+      <c r="E18" s="78"/>
+      <c r="F18" s="78"/>
+      <c r="G18" s="78"/>
+      <c r="H18" s="78"/>
+      <c r="I18" s="78"/>
+      <c r="J18" s="78"/>
+      <c r="K18" s="78"/>
+      <c r="L18" s="78"/>
+      <c r="M18" s="78"/>
+      <c r="N18" s="78"/>
+      <c r="O18" s="78"/>
+      <c r="P18" s="78"/>
+      <c r="Q18" s="79"/>
     </row>
     <row r="19" spans="1:17" ht="14.5" x14ac:dyDescent="0.25">
-      <c r="A19" s="79" t="s">
+      <c r="A19" s="68" t="s">
         <v>31</v>
       </c>
-      <c r="B19" s="80"/>
-      <c r="C19" s="80"/>
-      <c r="D19" s="80"/>
-      <c r="E19" s="80"/>
-      <c r="F19" s="80"/>
-      <c r="G19" s="80"/>
-      <c r="H19" s="80"/>
-      <c r="I19" s="80"/>
-      <c r="J19" s="80"/>
-      <c r="K19" s="80"/>
-      <c r="L19" s="80"/>
-      <c r="M19" s="80"/>
-      <c r="N19" s="80"/>
-      <c r="O19" s="80"/>
-      <c r="P19" s="80"/>
-      <c r="Q19" s="81"/>
+      <c r="B19" s="69"/>
+      <c r="C19" s="69"/>
+      <c r="D19" s="69"/>
+      <c r="E19" s="69"/>
+      <c r="F19" s="69"/>
+      <c r="G19" s="69"/>
+      <c r="H19" s="69"/>
+      <c r="I19" s="69"/>
+      <c r="J19" s="69"/>
+      <c r="K19" s="69"/>
+      <c r="L19" s="69"/>
+      <c r="M19" s="69"/>
+      <c r="N19" s="69"/>
+      <c r="O19" s="69"/>
+      <c r="P19" s="69"/>
+      <c r="Q19" s="70"/>
     </row>
     <row r="20" spans="1:17" ht="13" x14ac:dyDescent="0.25">
       <c r="A20" s="36">
         <v>1</v>
       </c>
-      <c r="B20" s="82" t="s">
+      <c r="B20" s="71" t="s">
         <v>32</v>
       </c>
-      <c r="C20" s="82"/>
-      <c r="D20" s="82"/>
-      <c r="E20" s="82"/>
-      <c r="F20" s="82"/>
-      <c r="G20" s="82"/>
-      <c r="H20" s="82"/>
-      <c r="I20" s="82"/>
-      <c r="J20" s="82"/>
-      <c r="K20" s="82"/>
-      <c r="L20" s="82"/>
-      <c r="M20" s="82"/>
-      <c r="N20" s="82"/>
-      <c r="O20" s="82"/>
-      <c r="P20" s="82"/>
-      <c r="Q20" s="83"/>
+      <c r="C20" s="71"/>
+      <c r="D20" s="71"/>
+      <c r="E20" s="71"/>
+      <c r="F20" s="71"/>
+      <c r="G20" s="71"/>
+      <c r="H20" s="71"/>
+      <c r="I20" s="71"/>
+      <c r="J20" s="71"/>
+      <c r="K20" s="71"/>
+      <c r="L20" s="71"/>
+      <c r="M20" s="71"/>
+      <c r="N20" s="71"/>
+      <c r="O20" s="71"/>
+      <c r="P20" s="71"/>
+      <c r="Q20" s="72"/>
     </row>
     <row r="21" spans="1:17" ht="13" x14ac:dyDescent="0.25">
       <c r="A21" s="36">
         <v>2</v>
       </c>
-      <c r="B21" s="84" t="s">
+      <c r="B21" s="73" t="s">
         <v>33</v>
       </c>
-      <c r="C21" s="85"/>
-      <c r="D21" s="85"/>
-      <c r="E21" s="85"/>
-      <c r="F21" s="85"/>
-      <c r="G21" s="85"/>
-      <c r="H21" s="85"/>
-      <c r="I21" s="85"/>
-      <c r="J21" s="85"/>
-      <c r="K21" s="85"/>
-      <c r="L21" s="85"/>
-      <c r="M21" s="85"/>
-      <c r="N21" s="85"/>
-      <c r="O21" s="85"/>
-      <c r="P21" s="85"/>
-      <c r="Q21" s="86"/>
+      <c r="C21" s="74"/>
+      <c r="D21" s="74"/>
+      <c r="E21" s="74"/>
+      <c r="F21" s="74"/>
+      <c r="G21" s="74"/>
+      <c r="H21" s="74"/>
+      <c r="I21" s="74"/>
+      <c r="J21" s="74"/>
+      <c r="K21" s="74"/>
+      <c r="L21" s="74"/>
+      <c r="M21" s="74"/>
+      <c r="N21" s="74"/>
+      <c r="O21" s="74"/>
+      <c r="P21" s="74"/>
+      <c r="Q21" s="75"/>
     </row>
     <row r="22" spans="1:17" ht="13" x14ac:dyDescent="0.25">
       <c r="A22" s="36">
         <v>3</v>
       </c>
-      <c r="B22" s="82" t="s">
+      <c r="B22" s="71" t="s">
         <v>34</v>
       </c>
-      <c r="C22" s="82"/>
-      <c r="D22" s="82"/>
-      <c r="E22" s="82"/>
-      <c r="F22" s="82"/>
-      <c r="G22" s="82"/>
-      <c r="H22" s="82"/>
-      <c r="I22" s="82"/>
-      <c r="J22" s="82"/>
-      <c r="K22" s="82"/>
-      <c r="L22" s="82"/>
-      <c r="M22" s="82"/>
-      <c r="N22" s="82"/>
-      <c r="O22" s="82"/>
-      <c r="P22" s="82"/>
-      <c r="Q22" s="83"/>
+      <c r="C22" s="71"/>
+      <c r="D22" s="71"/>
+      <c r="E22" s="71"/>
+      <c r="F22" s="71"/>
+      <c r="G22" s="71"/>
+      <c r="H22" s="71"/>
+      <c r="I22" s="71"/>
+      <c r="J22" s="71"/>
+      <c r="K22" s="71"/>
+      <c r="L22" s="71"/>
+      <c r="M22" s="71"/>
+      <c r="N22" s="71"/>
+      <c r="O22" s="71"/>
+      <c r="P22" s="71"/>
+      <c r="Q22" s="72"/>
     </row>
     <row r="23" spans="1:17" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="37">
         <v>4</v>
       </c>
-      <c r="B23" s="87" t="s">
+      <c r="B23" s="76" t="s">
         <v>35</v>
       </c>
-      <c r="C23" s="87"/>
-      <c r="D23" s="87"/>
-      <c r="E23" s="87"/>
-      <c r="F23" s="87"/>
-      <c r="G23" s="87"/>
-      <c r="H23" s="87"/>
-      <c r="I23" s="87"/>
-      <c r="J23" s="87"/>
-      <c r="K23" s="87"/>
-      <c r="L23" s="87"/>
-      <c r="M23" s="87"/>
-      <c r="N23" s="87"/>
-      <c r="O23" s="87"/>
-      <c r="P23" s="87"/>
-      <c r="Q23" s="88"/>
+      <c r="C23" s="76"/>
+      <c r="D23" s="76"/>
+      <c r="E23" s="76"/>
+      <c r="F23" s="76"/>
+      <c r="G23" s="76"/>
+      <c r="H23" s="76"/>
+      <c r="I23" s="76"/>
+      <c r="J23" s="76"/>
+      <c r="K23" s="76"/>
+      <c r="L23" s="76"/>
+      <c r="M23" s="76"/>
+      <c r="N23" s="76"/>
+      <c r="O23" s="76"/>
+      <c r="P23" s="76"/>
+      <c r="Q23" s="77"/>
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="A19:Q19"/>
-    <mergeCell ref="B20:Q20"/>
-    <mergeCell ref="B21:Q21"/>
-    <mergeCell ref="B22:Q22"/>
-    <mergeCell ref="B23:Q23"/>
+    <mergeCell ref="B6:Q6"/>
+    <mergeCell ref="A1:Q1"/>
+    <mergeCell ref="B2:Q2"/>
+    <mergeCell ref="B3:Q3"/>
+    <mergeCell ref="B4:Q4"/>
+    <mergeCell ref="B5:Q5"/>
     <mergeCell ref="B18:Q18"/>
     <mergeCell ref="B7:Q7"/>
     <mergeCell ref="B8:Q8"/>
@@ -3897,12 +3898,11 @@
     <mergeCell ref="B15:Q15"/>
     <mergeCell ref="B16:Q16"/>
     <mergeCell ref="B17:Q17"/>
-    <mergeCell ref="B6:Q6"/>
-    <mergeCell ref="A1:Q1"/>
-    <mergeCell ref="B2:Q2"/>
-    <mergeCell ref="B3:Q3"/>
-    <mergeCell ref="B4:Q4"/>
-    <mergeCell ref="B5:Q5"/>
+    <mergeCell ref="A19:Q19"/>
+    <mergeCell ref="B20:Q20"/>
+    <mergeCell ref="B21:Q21"/>
+    <mergeCell ref="B22:Q22"/>
+    <mergeCell ref="B23:Q23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="43" orientation="portrait" horizontalDpi="300" r:id="rId1"/>
@@ -3941,26 +3941,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="89" t="s">
+      <c r="A1" s="102" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="90"/>
-      <c r="C1" s="90"/>
-      <c r="D1" s="90"/>
-      <c r="E1" s="90"/>
-      <c r="F1" s="90"/>
-      <c r="G1" s="90"/>
-      <c r="H1" s="90"/>
-      <c r="I1" s="90"/>
-      <c r="J1" s="90"/>
-      <c r="K1" s="90"/>
-      <c r="L1" s="90"/>
-      <c r="M1" s="90"/>
-      <c r="N1" s="90"/>
-      <c r="O1" s="90"/>
-      <c r="P1" s="90"/>
-      <c r="Q1" s="90"/>
-      <c r="R1" s="91"/>
+      <c r="B1" s="103"/>
+      <c r="C1" s="103"/>
+      <c r="D1" s="103"/>
+      <c r="E1" s="103"/>
+      <c r="F1" s="103"/>
+      <c r="G1" s="103"/>
+      <c r="H1" s="103"/>
+      <c r="I1" s="103"/>
+      <c r="J1" s="103"/>
+      <c r="K1" s="103"/>
+      <c r="L1" s="103"/>
+      <c r="M1" s="103"/>
+      <c r="N1" s="103"/>
+      <c r="O1" s="103"/>
+      <c r="P1" s="103"/>
+      <c r="Q1" s="103"/>
+      <c r="R1" s="104"/>
     </row>
     <row r="2" spans="1:20" ht="50.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="27" t="s">
@@ -4073,26 +4073,26 @@
       </c>
     </row>
     <row r="4" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="92" t="s">
+      <c r="A4" s="105" t="s">
         <v>61</v>
       </c>
-      <c r="B4" s="93"/>
-      <c r="C4" s="93"/>
-      <c r="D4" s="93"/>
-      <c r="E4" s="93"/>
-      <c r="F4" s="93"/>
-      <c r="G4" s="93"/>
-      <c r="H4" s="93"/>
-      <c r="I4" s="93"/>
-      <c r="J4" s="93"/>
-      <c r="K4" s="93"/>
-      <c r="L4" s="93"/>
-      <c r="M4" s="93"/>
-      <c r="N4" s="93"/>
-      <c r="O4" s="93"/>
-      <c r="P4" s="93"/>
-      <c r="Q4" s="93"/>
-      <c r="R4" s="94"/>
+      <c r="B4" s="106"/>
+      <c r="C4" s="106"/>
+      <c r="D4" s="106"/>
+      <c r="E4" s="106"/>
+      <c r="F4" s="106"/>
+      <c r="G4" s="106"/>
+      <c r="H4" s="106"/>
+      <c r="I4" s="106"/>
+      <c r="J4" s="106"/>
+      <c r="K4" s="106"/>
+      <c r="L4" s="106"/>
+      <c r="M4" s="106"/>
+      <c r="N4" s="106"/>
+      <c r="O4" s="106"/>
+      <c r="P4" s="106"/>
+      <c r="Q4" s="106"/>
+      <c r="R4" s="107"/>
     </row>
     <row r="5" spans="1:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="95" t="s">
@@ -4101,22 +4101,22 @@
       <c r="B5" s="96"/>
       <c r="C5" s="97"/>
       <c r="D5" s="38"/>
-      <c r="E5" s="98" t="s">
+      <c r="E5" s="89" t="s">
         <v>63</v>
       </c>
-      <c r="F5" s="99"/>
-      <c r="G5" s="99"/>
-      <c r="H5" s="99"/>
-      <c r="I5" s="99"/>
-      <c r="J5" s="99"/>
-      <c r="K5" s="99"/>
-      <c r="L5" s="99"/>
-      <c r="M5" s="99"/>
-      <c r="N5" s="99"/>
-      <c r="O5" s="99"/>
-      <c r="P5" s="99"/>
-      <c r="Q5" s="99"/>
-      <c r="R5" s="100"/>
+      <c r="F5" s="90"/>
+      <c r="G5" s="90"/>
+      <c r="H5" s="90"/>
+      <c r="I5" s="90"/>
+      <c r="J5" s="90"/>
+      <c r="K5" s="90"/>
+      <c r="L5" s="90"/>
+      <c r="M5" s="90"/>
+      <c r="N5" s="90"/>
+      <c r="O5" s="90"/>
+      <c r="P5" s="90"/>
+      <c r="Q5" s="90"/>
+      <c r="R5" s="91"/>
       <c r="T5" s="24">
         <v>3</v>
       </c>
@@ -4139,31 +4139,31 @@
       <c r="O6" s="96"/>
       <c r="P6" s="96"/>
       <c r="Q6" s="96"/>
-      <c r="R6" s="101"/>
+      <c r="R6" s="98"/>
     </row>
     <row r="7" spans="1:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="102" t="s">
+      <c r="A7" s="92" t="s">
         <v>64</v>
       </c>
-      <c r="B7" s="103"/>
-      <c r="C7" s="104"/>
+      <c r="B7" s="93"/>
+      <c r="C7" s="94"/>
       <c r="D7" s="38"/>
-      <c r="E7" s="98" t="s">
+      <c r="E7" s="89" t="s">
         <v>63</v>
       </c>
-      <c r="F7" s="99"/>
-      <c r="G7" s="99"/>
-      <c r="H7" s="99"/>
-      <c r="I7" s="99"/>
-      <c r="J7" s="99"/>
-      <c r="K7" s="99"/>
-      <c r="L7" s="99"/>
-      <c r="M7" s="99"/>
-      <c r="N7" s="99"/>
-      <c r="O7" s="99"/>
-      <c r="P7" s="99"/>
-      <c r="Q7" s="99"/>
-      <c r="R7" s="100"/>
+      <c r="F7" s="90"/>
+      <c r="G7" s="90"/>
+      <c r="H7" s="90"/>
+      <c r="I7" s="90"/>
+      <c r="J7" s="90"/>
+      <c r="K7" s="90"/>
+      <c r="L7" s="90"/>
+      <c r="M7" s="90"/>
+      <c r="N7" s="90"/>
+      <c r="O7" s="90"/>
+      <c r="P7" s="90"/>
+      <c r="Q7" s="90"/>
+      <c r="R7" s="91"/>
     </row>
     <row r="8" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="95"/>
@@ -4183,7 +4183,7 @@
       <c r="O8" s="96"/>
       <c r="P8" s="96"/>
       <c r="Q8" s="96"/>
-      <c r="R8" s="101"/>
+      <c r="R8" s="98"/>
     </row>
     <row r="9" spans="1:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="95" t="s">
@@ -4192,22 +4192,22 @@
       <c r="B9" s="96"/>
       <c r="C9" s="97"/>
       <c r="D9" s="38"/>
-      <c r="E9" s="98" t="s">
+      <c r="E9" s="89" t="s">
         <v>63</v>
       </c>
-      <c r="F9" s="99"/>
-      <c r="G9" s="99"/>
-      <c r="H9" s="99"/>
-      <c r="I9" s="99"/>
-      <c r="J9" s="99"/>
-      <c r="K9" s="99"/>
-      <c r="L9" s="99"/>
-      <c r="M9" s="99"/>
-      <c r="N9" s="99"/>
-      <c r="O9" s="99"/>
-      <c r="P9" s="99"/>
-      <c r="Q9" s="99"/>
-      <c r="R9" s="100"/>
+      <c r="F9" s="90"/>
+      <c r="G9" s="90"/>
+      <c r="H9" s="90"/>
+      <c r="I9" s="90"/>
+      <c r="J9" s="90"/>
+      <c r="K9" s="90"/>
+      <c r="L9" s="90"/>
+      <c r="M9" s="90"/>
+      <c r="N9" s="90"/>
+      <c r="O9" s="90"/>
+      <c r="P9" s="90"/>
+      <c r="Q9" s="90"/>
+      <c r="R9" s="91"/>
     </row>
     <row r="10" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="95"/>
@@ -4227,7 +4227,7 @@
       <c r="O10" s="96"/>
       <c r="P10" s="96"/>
       <c r="Q10" s="96"/>
-      <c r="R10" s="101"/>
+      <c r="R10" s="98"/>
     </row>
     <row r="11" spans="1:20" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="95" t="s">
@@ -4236,22 +4236,22 @@
       <c r="B11" s="96"/>
       <c r="C11" s="97"/>
       <c r="D11" s="38"/>
-      <c r="E11" s="98" t="s">
+      <c r="E11" s="89" t="s">
         <v>67</v>
       </c>
-      <c r="F11" s="99"/>
-      <c r="G11" s="99"/>
-      <c r="H11" s="99"/>
-      <c r="I11" s="99"/>
-      <c r="J11" s="99"/>
-      <c r="K11" s="99"/>
-      <c r="L11" s="99"/>
-      <c r="M11" s="99"/>
-      <c r="N11" s="99"/>
-      <c r="O11" s="99"/>
-      <c r="P11" s="99"/>
-      <c r="Q11" s="99"/>
-      <c r="R11" s="100"/>
+      <c r="F11" s="90"/>
+      <c r="G11" s="90"/>
+      <c r="H11" s="90"/>
+      <c r="I11" s="90"/>
+      <c r="J11" s="90"/>
+      <c r="K11" s="90"/>
+      <c r="L11" s="90"/>
+      <c r="M11" s="90"/>
+      <c r="N11" s="90"/>
+      <c r="O11" s="90"/>
+      <c r="P11" s="90"/>
+      <c r="Q11" s="90"/>
+      <c r="R11" s="91"/>
     </row>
     <row r="12" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="95" t="s">
@@ -4273,7 +4273,7 @@
       <c r="O12" s="96"/>
       <c r="P12" s="96"/>
       <c r="Q12" s="96"/>
-      <c r="R12" s="101"/>
+      <c r="R12" s="98"/>
     </row>
     <row r="13" spans="1:20" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="25">
@@ -4285,26 +4285,31 @@
       <c r="C13" s="26" t="s">
         <v>97</v>
       </c>
-      <c r="D13" s="105" t="s">
+      <c r="D13" s="99" t="s">
         <v>70</v>
       </c>
-      <c r="E13" s="106"/>
-      <c r="F13" s="106"/>
-      <c r="G13" s="106"/>
-      <c r="H13" s="106"/>
-      <c r="I13" s="106"/>
-      <c r="J13" s="106"/>
-      <c r="K13" s="106"/>
-      <c r="L13" s="106"/>
-      <c r="M13" s="106"/>
-      <c r="N13" s="106"/>
-      <c r="O13" s="106"/>
-      <c r="P13" s="106"/>
-      <c r="Q13" s="106"/>
-      <c r="R13" s="107"/>
+      <c r="E13" s="100"/>
+      <c r="F13" s="100"/>
+      <c r="G13" s="100"/>
+      <c r="H13" s="100"/>
+      <c r="I13" s="100"/>
+      <c r="J13" s="100"/>
+      <c r="K13" s="100"/>
+      <c r="L13" s="100"/>
+      <c r="M13" s="100"/>
+      <c r="N13" s="100"/>
+      <c r="O13" s="100"/>
+      <c r="P13" s="100"/>
+      <c r="Q13" s="100"/>
+      <c r="R13" s="101"/>
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A1:R1"/>
+    <mergeCell ref="A4:R4"/>
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="E5:R5"/>
+    <mergeCell ref="A6:R6"/>
     <mergeCell ref="E7:R7"/>
     <mergeCell ref="A7:C7"/>
     <mergeCell ref="A11:C11"/>
@@ -4315,11 +4320,6 @@
     <mergeCell ref="A9:C9"/>
     <mergeCell ref="E9:R9"/>
     <mergeCell ref="A10:R10"/>
-    <mergeCell ref="A1:R1"/>
-    <mergeCell ref="A4:R4"/>
-    <mergeCell ref="A5:C5"/>
-    <mergeCell ref="E5:R5"/>
-    <mergeCell ref="A6:R6"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup scale="28" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -4328,11 +4328,10 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="896f6421-0ffe-4cdf-9397-f39e719ecdb4" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<titus xmlns="http://schemas.titus.com/TitusProperties/">
+  <TitusGUID xmlns="">b32b142f-e1a3-4636-987f-842931850c11</TitusGUID>
+  <TitusMetadata xmlns="">eyJucyI6Imh0dHA6XC9cL3d3dy50aXR1cy5jb21cL25zXC9UVExUSVRVUyIsInByb3BzIjpbeyJuIjoiQ2xhc3NpZmljYXRpb24iLCJ2YWxzIjpbeyJ2YWx1ZSI6IkludGVybmFsIn1dfV19</TitusMetadata>
+</titus>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4577,10 +4576,11 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<titus xmlns="http://schemas.titus.com/TitusProperties/">
-  <TitusGUID xmlns="">b32b142f-e1a3-4636-987f-842931850c11</TitusGUID>
-  <TitusMetadata xmlns="">eyJucyI6Imh0dHA6XC9cL3d3dy50aXR1cy5jb21cL25zXC9UVExUSVRVUyIsInByb3BzIjpbeyJuIjoiQ2xhc3NpZmljYXRpb24iLCJ2YWxzIjpbeyJ2YWx1ZSI6IkludGVybmFsIn1dfV19</TitusMetadata>
-</titus>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="896f6421-0ffe-4cdf-9397-f39e719ecdb4" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4593,18 +4593,10 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EC96BEBB-37FE-4C78-B1A0-F4825207DA4D}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A3EF0A4F-E3E9-4C94-9786-69F046D3300A}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="896f6421-0ffe-4cdf-9397-f39e719ecdb4"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="47b22ed6-09de-4eef-8e70-1f7bccb8aa81"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.titus.com/TitusProperties/"/>
+    <ds:schemaRef ds:uri=""/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -4629,10 +4621,18 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A3EF0A4F-E3E9-4C94-9786-69F046D3300A}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EC96BEBB-37FE-4C78-B1A0-F4825207DA4D}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.titus.com/TitusProperties/"/>
-    <ds:schemaRef ds:uri=""/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="896f6421-0ffe-4cdf-9397-f39e719ecdb4"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="47b22ed6-09de-4eef-8e70-1f7bccb8aa81"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Local isolator changes completed
</commit_message>
<xml_diff>
--- a/thermax_backend/templates/enviro_load_list_template.xlsx
+++ b/thermax_backend/templates/enviro_load_list_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\abhishekraje30\frappe-bench\apps\thermax_backend\thermax_backend\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C0A61D7-574B-40A8-9399-9E5C2F69A0F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{583903CF-DC96-429E-B010-A5A71585DD92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="678" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="678" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="COVER" sheetId="9" r:id="rId1"/>
@@ -1383,6 +1383,42 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="39" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="40" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1434,41 +1470,38 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="38" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="39" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="40" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="13" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="14" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1500,38 +1533,32 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="18" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="13" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="14" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1542,6 +1569,9 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1551,18 +1581,6 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1570,24 +1588,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1686,15 +1686,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>1085850</xdr:colOff>
+      <xdr:colOff>1584779</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
+      <xdr:rowOff>171904</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>2762250</xdr:colOff>
+      <xdr:colOff>3261179</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>1343025</xdr:rowOff>
+      <xdr:rowOff>1333954</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1724,7 +1724,7 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="3638550" y="180975"/>
+          <a:off x="4260850" y="171904"/>
           <a:ext cx="1676400" cy="1162050"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2280,8 +2280,8 @@
   </sheetPr>
   <dimension ref="A1:CD35"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" topLeftCell="A2" zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="70" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10:G10"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="70" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6:G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.3"/>
@@ -2929,50 +2929,50 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="116.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="39"/>
-      <c r="B1" s="40"/>
-      <c r="C1" s="40"/>
-      <c r="D1" s="40"/>
-      <c r="E1" s="40"/>
-      <c r="F1" s="40"/>
-      <c r="G1" s="40"/>
-      <c r="H1" s="41"/>
+      <c r="A1" s="51"/>
+      <c r="B1" s="52"/>
+      <c r="C1" s="52"/>
+      <c r="D1" s="52"/>
+      <c r="E1" s="52"/>
+      <c r="F1" s="52"/>
+      <c r="G1" s="52"/>
+      <c r="H1" s="53"/>
     </row>
     <row r="2" spans="1:8" ht="26.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="42" t="s">
+      <c r="A2" s="54" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="43"/>
-      <c r="C2" s="43"/>
-      <c r="D2" s="43"/>
-      <c r="E2" s="43"/>
-      <c r="F2" s="43"/>
-      <c r="G2" s="43"/>
-      <c r="H2" s="44"/>
+      <c r="B2" s="55"/>
+      <c r="C2" s="55"/>
+      <c r="D2" s="55"/>
+      <c r="E2" s="55"/>
+      <c r="F2" s="55"/>
+      <c r="G2" s="55"/>
+      <c r="H2" s="56"/>
     </row>
     <row r="3" spans="1:8" ht="23.5" x14ac:dyDescent="0.3">
-      <c r="A3" s="45" t="s">
+      <c r="A3" s="57" t="s">
         <v>74</v>
       </c>
-      <c r="B3" s="46"/>
-      <c r="C3" s="46"/>
-      <c r="D3" s="46"/>
-      <c r="E3" s="46"/>
-      <c r="F3" s="46"/>
-      <c r="G3" s="46"/>
-      <c r="H3" s="47"/>
+      <c r="B3" s="58"/>
+      <c r="C3" s="58"/>
+      <c r="D3" s="58"/>
+      <c r="E3" s="58"/>
+      <c r="F3" s="58"/>
+      <c r="G3" s="58"/>
+      <c r="H3" s="59"/>
     </row>
     <row r="4" spans="1:8" ht="24" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="48" t="s">
+      <c r="A4" s="60" t="s">
         <v>73</v>
       </c>
-      <c r="B4" s="49"/>
-      <c r="C4" s="49"/>
-      <c r="D4" s="49"/>
-      <c r="E4" s="49"/>
-      <c r="F4" s="49"/>
-      <c r="G4" s="49"/>
-      <c r="H4" s="50"/>
+      <c r="B4" s="61"/>
+      <c r="C4" s="61"/>
+      <c r="D4" s="61"/>
+      <c r="E4" s="61"/>
+      <c r="F4" s="61"/>
+      <c r="G4" s="61"/>
+      <c r="H4" s="62"/>
     </row>
     <row r="5" spans="1:8" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="4"/>
@@ -2986,76 +2986,76 @@
     </row>
     <row r="6" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4"/>
-      <c r="B6" s="51" t="s">
+      <c r="B6" s="63" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="52"/>
-      <c r="D6" s="53" t="s">
+      <c r="C6" s="64"/>
+      <c r="D6" s="65" t="s">
         <v>2</v>
       </c>
-      <c r="E6" s="54"/>
-      <c r="F6" s="54"/>
-      <c r="G6" s="55"/>
+      <c r="E6" s="66"/>
+      <c r="F6" s="66"/>
+      <c r="G6" s="67"/>
       <c r="H6" s="6"/>
     </row>
     <row r="7" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="4"/>
-      <c r="B7" s="66" t="s">
+      <c r="B7" s="49" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="67"/>
-      <c r="D7" s="58"/>
-      <c r="E7" s="59"/>
-      <c r="F7" s="59"/>
-      <c r="G7" s="60"/>
+      <c r="C7" s="50"/>
+      <c r="D7" s="41"/>
+      <c r="E7" s="42"/>
+      <c r="F7" s="42"/>
+      <c r="G7" s="43"/>
       <c r="H7" s="6"/>
     </row>
     <row r="8" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4"/>
-      <c r="B8" s="56" t="s">
+      <c r="B8" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="57"/>
-      <c r="D8" s="58"/>
-      <c r="E8" s="59"/>
-      <c r="F8" s="59"/>
-      <c r="G8" s="60"/>
+      <c r="C8" s="40"/>
+      <c r="D8" s="41"/>
+      <c r="E8" s="42"/>
+      <c r="F8" s="42"/>
+      <c r="G8" s="43"/>
       <c r="H8" s="6"/>
     </row>
     <row r="9" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="4"/>
-      <c r="B9" s="56" t="s">
+      <c r="B9" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="57"/>
-      <c r="D9" s="58"/>
-      <c r="E9" s="59"/>
-      <c r="F9" s="59"/>
-      <c r="G9" s="60"/>
+      <c r="C9" s="40"/>
+      <c r="D9" s="41"/>
+      <c r="E9" s="42"/>
+      <c r="F9" s="42"/>
+      <c r="G9" s="43"/>
       <c r="H9" s="6"/>
     </row>
     <row r="10" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="4"/>
-      <c r="B10" s="56" t="s">
+      <c r="B10" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="57"/>
-      <c r="D10" s="58"/>
-      <c r="E10" s="59"/>
-      <c r="F10" s="59"/>
-      <c r="G10" s="60"/>
+      <c r="C10" s="40"/>
+      <c r="D10" s="41"/>
+      <c r="E10" s="42"/>
+      <c r="F10" s="42"/>
+      <c r="G10" s="43"/>
       <c r="H10" s="6"/>
     </row>
     <row r="11" spans="1:8" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="4"/>
-      <c r="B11" s="61" t="s">
+      <c r="B11" s="44" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="62"/>
-      <c r="D11" s="63"/>
-      <c r="E11" s="64"/>
-      <c r="F11" s="64"/>
-      <c r="G11" s="65"/>
+      <c r="C11" s="45"/>
+      <c r="D11" s="46"/>
+      <c r="E11" s="47"/>
+      <c r="F11" s="47"/>
+      <c r="G11" s="48"/>
       <c r="H11" s="6"/>
     </row>
     <row r="12" spans="1:8" s="9" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -3319,6 +3319,12 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A2:H2"/>
+    <mergeCell ref="A3:H3"/>
+    <mergeCell ref="A4:H4"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="D6:G6"/>
     <mergeCell ref="B10:C10"/>
     <mergeCell ref="D10:G10"/>
     <mergeCell ref="B11:C11"/>
@@ -3329,12 +3335,6 @@
     <mergeCell ref="D8:G8"/>
     <mergeCell ref="B9:C9"/>
     <mergeCell ref="D9:G9"/>
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="A2:H2"/>
-    <mergeCell ref="A3:H3"/>
-    <mergeCell ref="A4:H4"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="D6:G6"/>
   </mergeCells>
   <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="66" fitToHeight="100" orientation="portrait" r:id="rId1"/>
@@ -3346,7 +3346,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Q23"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="90" zoomScaleNormal="100" zoomScaleSheetLayoutView="90" workbookViewId="0">
+    <sheetView view="pageBreakPreview" zoomScale="90" zoomScaleNormal="100" zoomScaleSheetLayoutView="90" workbookViewId="0">
       <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
@@ -3358,534 +3358,533 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="86" t="s">
+      <c r="A1" s="70" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="87"/>
-      <c r="C1" s="87"/>
-      <c r="D1" s="87"/>
-      <c r="E1" s="87"/>
-      <c r="F1" s="87"/>
-      <c r="G1" s="87"/>
-      <c r="H1" s="87"/>
-      <c r="I1" s="87"/>
-      <c r="J1" s="87"/>
-      <c r="K1" s="87"/>
-      <c r="L1" s="87"/>
-      <c r="M1" s="87"/>
-      <c r="N1" s="87"/>
-      <c r="O1" s="87"/>
-      <c r="P1" s="87"/>
-      <c r="Q1" s="88"/>
+      <c r="B1" s="71"/>
+      <c r="C1" s="71"/>
+      <c r="D1" s="71"/>
+      <c r="E1" s="71"/>
+      <c r="F1" s="71"/>
+      <c r="G1" s="71"/>
+      <c r="H1" s="71"/>
+      <c r="I1" s="71"/>
+      <c r="J1" s="71"/>
+      <c r="K1" s="71"/>
+      <c r="L1" s="71"/>
+      <c r="M1" s="71"/>
+      <c r="N1" s="71"/>
+      <c r="O1" s="71"/>
+      <c r="P1" s="71"/>
+      <c r="Q1" s="72"/>
     </row>
     <row r="2" spans="1:17" ht="13" x14ac:dyDescent="0.25">
       <c r="A2" s="34" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="84" t="s">
+      <c r="B2" s="73" t="s">
         <v>81</v>
       </c>
-      <c r="C2" s="84"/>
-      <c r="D2" s="84"/>
-      <c r="E2" s="84"/>
-      <c r="F2" s="84"/>
-      <c r="G2" s="84"/>
-      <c r="H2" s="84"/>
-      <c r="I2" s="84"/>
-      <c r="J2" s="84"/>
-      <c r="K2" s="84"/>
-      <c r="L2" s="84"/>
-      <c r="M2" s="84"/>
-      <c r="N2" s="84"/>
-      <c r="O2" s="84"/>
-      <c r="P2" s="84"/>
-      <c r="Q2" s="85"/>
+      <c r="C2" s="73"/>
+      <c r="D2" s="73"/>
+      <c r="E2" s="73"/>
+      <c r="F2" s="73"/>
+      <c r="G2" s="73"/>
+      <c r="H2" s="73"/>
+      <c r="I2" s="73"/>
+      <c r="J2" s="73"/>
+      <c r="K2" s="73"/>
+      <c r="L2" s="73"/>
+      <c r="M2" s="73"/>
+      <c r="N2" s="73"/>
+      <c r="O2" s="73"/>
+      <c r="P2" s="73"/>
+      <c r="Q2" s="74"/>
     </row>
     <row r="3" spans="1:17" ht="13" x14ac:dyDescent="0.25">
       <c r="A3" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="84" t="s">
+      <c r="B3" s="73" t="s">
         <v>82</v>
       </c>
-      <c r="C3" s="84"/>
-      <c r="D3" s="84"/>
-      <c r="E3" s="84"/>
-      <c r="F3" s="84"/>
-      <c r="G3" s="84"/>
-      <c r="H3" s="84"/>
-      <c r="I3" s="84"/>
-      <c r="J3" s="84"/>
-      <c r="K3" s="84"/>
-      <c r="L3" s="84"/>
-      <c r="M3" s="84"/>
-      <c r="N3" s="84"/>
-      <c r="O3" s="84"/>
-      <c r="P3" s="84"/>
-      <c r="Q3" s="85"/>
+      <c r="C3" s="73"/>
+      <c r="D3" s="73"/>
+      <c r="E3" s="73"/>
+      <c r="F3" s="73"/>
+      <c r="G3" s="73"/>
+      <c r="H3" s="73"/>
+      <c r="I3" s="73"/>
+      <c r="J3" s="73"/>
+      <c r="K3" s="73"/>
+      <c r="L3" s="73"/>
+      <c r="M3" s="73"/>
+      <c r="N3" s="73"/>
+      <c r="O3" s="73"/>
+      <c r="P3" s="73"/>
+      <c r="Q3" s="74"/>
     </row>
     <row r="4" spans="1:17" ht="13" x14ac:dyDescent="0.25">
       <c r="A4" s="34" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="84" t="s">
+      <c r="B4" s="73" t="s">
         <v>83</v>
       </c>
-      <c r="C4" s="84"/>
-      <c r="D4" s="84"/>
-      <c r="E4" s="84"/>
-      <c r="F4" s="84"/>
-      <c r="G4" s="84"/>
-      <c r="H4" s="84"/>
-      <c r="I4" s="84"/>
-      <c r="J4" s="84"/>
-      <c r="K4" s="84"/>
-      <c r="L4" s="84"/>
-      <c r="M4" s="84"/>
-      <c r="N4" s="84"/>
-      <c r="O4" s="84"/>
-      <c r="P4" s="84"/>
-      <c r="Q4" s="85"/>
+      <c r="C4" s="73"/>
+      <c r="D4" s="73"/>
+      <c r="E4" s="73"/>
+      <c r="F4" s="73"/>
+      <c r="G4" s="73"/>
+      <c r="H4" s="73"/>
+      <c r="I4" s="73"/>
+      <c r="J4" s="73"/>
+      <c r="K4" s="73"/>
+      <c r="L4" s="73"/>
+      <c r="M4" s="73"/>
+      <c r="N4" s="73"/>
+      <c r="O4" s="73"/>
+      <c r="P4" s="73"/>
+      <c r="Q4" s="74"/>
     </row>
     <row r="5" spans="1:17" ht="13" x14ac:dyDescent="0.25">
       <c r="A5" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="84" t="s">
+      <c r="B5" s="73" t="s">
         <v>84</v>
       </c>
-      <c r="C5" s="84"/>
-      <c r="D5" s="84"/>
-      <c r="E5" s="84"/>
-      <c r="F5" s="84"/>
-      <c r="G5" s="84"/>
-      <c r="H5" s="84"/>
-      <c r="I5" s="84"/>
-      <c r="J5" s="84"/>
-      <c r="K5" s="84"/>
-      <c r="L5" s="84"/>
-      <c r="M5" s="84"/>
-      <c r="N5" s="84"/>
-      <c r="O5" s="84"/>
-      <c r="P5" s="84"/>
-      <c r="Q5" s="85"/>
+      <c r="C5" s="73"/>
+      <c r="D5" s="73"/>
+      <c r="E5" s="73"/>
+      <c r="F5" s="73"/>
+      <c r="G5" s="73"/>
+      <c r="H5" s="73"/>
+      <c r="I5" s="73"/>
+      <c r="J5" s="73"/>
+      <c r="K5" s="73"/>
+      <c r="L5" s="73"/>
+      <c r="M5" s="73"/>
+      <c r="N5" s="73"/>
+      <c r="O5" s="73"/>
+      <c r="P5" s="73"/>
+      <c r="Q5" s="74"/>
     </row>
     <row r="6" spans="1:17" ht="13" x14ac:dyDescent="0.25">
       <c r="A6" s="34" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="80" t="s">
+      <c r="B6" s="68" t="s">
         <v>85</v>
       </c>
-      <c r="C6" s="80"/>
-      <c r="D6" s="80"/>
-      <c r="E6" s="80"/>
-      <c r="F6" s="80"/>
-      <c r="G6" s="80"/>
-      <c r="H6" s="80"/>
-      <c r="I6" s="80"/>
-      <c r="J6" s="80"/>
-      <c r="K6" s="80"/>
-      <c r="L6" s="80"/>
-      <c r="M6" s="80"/>
-      <c r="N6" s="80"/>
-      <c r="O6" s="80"/>
-      <c r="P6" s="80"/>
-      <c r="Q6" s="81"/>
+      <c r="C6" s="68"/>
+      <c r="D6" s="68"/>
+      <c r="E6" s="68"/>
+      <c r="F6" s="68"/>
+      <c r="G6" s="68"/>
+      <c r="H6" s="68"/>
+      <c r="I6" s="68"/>
+      <c r="J6" s="68"/>
+      <c r="K6" s="68"/>
+      <c r="L6" s="68"/>
+      <c r="M6" s="68"/>
+      <c r="N6" s="68"/>
+      <c r="O6" s="68"/>
+      <c r="P6" s="68"/>
+      <c r="Q6" s="69"/>
     </row>
     <row r="7" spans="1:17" ht="13" x14ac:dyDescent="0.25">
       <c r="A7" s="34" t="s">
         <v>21</v>
       </c>
-      <c r="B7" s="80" t="s">
+      <c r="B7" s="68" t="s">
         <v>86</v>
       </c>
-      <c r="C7" s="80"/>
-      <c r="D7" s="80"/>
-      <c r="E7" s="80"/>
-      <c r="F7" s="80"/>
-      <c r="G7" s="80"/>
-      <c r="H7" s="80"/>
-      <c r="I7" s="80"/>
-      <c r="J7" s="80"/>
-      <c r="K7" s="80"/>
-      <c r="L7" s="80"/>
-      <c r="M7" s="80"/>
-      <c r="N7" s="80"/>
-      <c r="O7" s="80"/>
-      <c r="P7" s="80"/>
-      <c r="Q7" s="81"/>
+      <c r="C7" s="68"/>
+      <c r="D7" s="68"/>
+      <c r="E7" s="68"/>
+      <c r="F7" s="68"/>
+      <c r="G7" s="68"/>
+      <c r="H7" s="68"/>
+      <c r="I7" s="68"/>
+      <c r="J7" s="68"/>
+      <c r="K7" s="68"/>
+      <c r="L7" s="68"/>
+      <c r="M7" s="68"/>
+      <c r="N7" s="68"/>
+      <c r="O7" s="68"/>
+      <c r="P7" s="68"/>
+      <c r="Q7" s="69"/>
     </row>
     <row r="8" spans="1:17" ht="13" x14ac:dyDescent="0.25">
       <c r="A8" s="34" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="80" t="s">
+      <c r="B8" s="68" t="s">
         <v>87</v>
       </c>
-      <c r="C8" s="80"/>
-      <c r="D8" s="80"/>
-      <c r="E8" s="80"/>
-      <c r="F8" s="80"/>
-      <c r="G8" s="80"/>
-      <c r="H8" s="80"/>
-      <c r="I8" s="80"/>
-      <c r="J8" s="80"/>
-      <c r="K8" s="80"/>
-      <c r="L8" s="80"/>
-      <c r="M8" s="80"/>
-      <c r="N8" s="80"/>
-      <c r="O8" s="80"/>
-      <c r="P8" s="80"/>
-      <c r="Q8" s="81"/>
+      <c r="C8" s="68"/>
+      <c r="D8" s="68"/>
+      <c r="E8" s="68"/>
+      <c r="F8" s="68"/>
+      <c r="G8" s="68"/>
+      <c r="H8" s="68"/>
+      <c r="I8" s="68"/>
+      <c r="J8" s="68"/>
+      <c r="K8" s="68"/>
+      <c r="L8" s="68"/>
+      <c r="M8" s="68"/>
+      <c r="N8" s="68"/>
+      <c r="O8" s="68"/>
+      <c r="P8" s="68"/>
+      <c r="Q8" s="69"/>
     </row>
     <row r="9" spans="1:17" ht="13" x14ac:dyDescent="0.25">
       <c r="A9" s="34" t="s">
         <v>23</v>
       </c>
-      <c r="B9" s="80" t="s">
+      <c r="B9" s="68" t="s">
         <v>88</v>
       </c>
-      <c r="C9" s="80"/>
-      <c r="D9" s="80"/>
-      <c r="E9" s="80"/>
-      <c r="F9" s="80"/>
-      <c r="G9" s="80"/>
-      <c r="H9" s="80"/>
-      <c r="I9" s="80"/>
-      <c r="J9" s="80"/>
-      <c r="K9" s="80"/>
-      <c r="L9" s="80"/>
-      <c r="M9" s="80"/>
-      <c r="N9" s="80"/>
-      <c r="O9" s="80"/>
-      <c r="P9" s="80"/>
-      <c r="Q9" s="81"/>
+      <c r="C9" s="68"/>
+      <c r="D9" s="68"/>
+      <c r="E9" s="68"/>
+      <c r="F9" s="68"/>
+      <c r="G9" s="68"/>
+      <c r="H9" s="68"/>
+      <c r="I9" s="68"/>
+      <c r="J9" s="68"/>
+      <c r="K9" s="68"/>
+      <c r="L9" s="68"/>
+      <c r="M9" s="68"/>
+      <c r="N9" s="68"/>
+      <c r="O9" s="68"/>
+      <c r="P9" s="68"/>
+      <c r="Q9" s="69"/>
     </row>
     <row r="10" spans="1:17" ht="13" x14ac:dyDescent="0.25">
       <c r="A10" s="34" t="s">
         <v>24</v>
       </c>
-      <c r="B10" s="80" t="s">
+      <c r="B10" s="68" t="s">
         <v>89</v>
       </c>
-      <c r="C10" s="80"/>
-      <c r="D10" s="80"/>
-      <c r="E10" s="80"/>
-      <c r="F10" s="80"/>
-      <c r="G10" s="80"/>
-      <c r="H10" s="80"/>
-      <c r="I10" s="80"/>
-      <c r="J10" s="80"/>
-      <c r="K10" s="80"/>
-      <c r="L10" s="80"/>
-      <c r="M10" s="80"/>
-      <c r="N10" s="80"/>
-      <c r="O10" s="80"/>
-      <c r="P10" s="80"/>
-      <c r="Q10" s="81"/>
+      <c r="C10" s="68"/>
+      <c r="D10" s="68"/>
+      <c r="E10" s="68"/>
+      <c r="F10" s="68"/>
+      <c r="G10" s="68"/>
+      <c r="H10" s="68"/>
+      <c r="I10" s="68"/>
+      <c r="J10" s="68"/>
+      <c r="K10" s="68"/>
+      <c r="L10" s="68"/>
+      <c r="M10" s="68"/>
+      <c r="N10" s="68"/>
+      <c r="O10" s="68"/>
+      <c r="P10" s="68"/>
+      <c r="Q10" s="69"/>
     </row>
     <row r="11" spans="1:17" ht="13" x14ac:dyDescent="0.25">
       <c r="A11" s="34" t="s">
         <v>25</v>
       </c>
-      <c r="B11" s="80" t="s">
+      <c r="B11" s="68" t="s">
         <v>90</v>
       </c>
-      <c r="C11" s="80"/>
-      <c r="D11" s="80"/>
-      <c r="E11" s="80"/>
-      <c r="F11" s="80"/>
-      <c r="G11" s="80"/>
-      <c r="H11" s="80"/>
-      <c r="I11" s="80"/>
-      <c r="J11" s="80"/>
-      <c r="K11" s="80"/>
-      <c r="L11" s="80"/>
-      <c r="M11" s="80"/>
-      <c r="N11" s="80"/>
-      <c r="O11" s="80"/>
-      <c r="P11" s="80"/>
-      <c r="Q11" s="81"/>
+      <c r="C11" s="68"/>
+      <c r="D11" s="68"/>
+      <c r="E11" s="68"/>
+      <c r="F11" s="68"/>
+      <c r="G11" s="68"/>
+      <c r="H11" s="68"/>
+      <c r="I11" s="68"/>
+      <c r="J11" s="68"/>
+      <c r="K11" s="68"/>
+      <c r="L11" s="68"/>
+      <c r="M11" s="68"/>
+      <c r="N11" s="68"/>
+      <c r="O11" s="68"/>
+      <c r="P11" s="68"/>
+      <c r="Q11" s="69"/>
     </row>
     <row r="12" spans="1:17" ht="13" x14ac:dyDescent="0.25">
       <c r="A12" s="34" t="s">
         <v>26</v>
       </c>
-      <c r="B12" s="80" t="s">
+      <c r="B12" s="68" t="s">
         <v>91</v>
       </c>
-      <c r="C12" s="80"/>
-      <c r="D12" s="80"/>
-      <c r="E12" s="80"/>
-      <c r="F12" s="80"/>
-      <c r="G12" s="80"/>
-      <c r="H12" s="80"/>
-      <c r="I12" s="80"/>
-      <c r="J12" s="80"/>
-      <c r="K12" s="80"/>
-      <c r="L12" s="80"/>
-      <c r="M12" s="80"/>
-      <c r="N12" s="80"/>
-      <c r="O12" s="80"/>
-      <c r="P12" s="80"/>
-      <c r="Q12" s="81"/>
+      <c r="C12" s="68"/>
+      <c r="D12" s="68"/>
+      <c r="E12" s="68"/>
+      <c r="F12" s="68"/>
+      <c r="G12" s="68"/>
+      <c r="H12" s="68"/>
+      <c r="I12" s="68"/>
+      <c r="J12" s="68"/>
+      <c r="K12" s="68"/>
+      <c r="L12" s="68"/>
+      <c r="M12" s="68"/>
+      <c r="N12" s="68"/>
+      <c r="O12" s="68"/>
+      <c r="P12" s="68"/>
+      <c r="Q12" s="69"/>
     </row>
     <row r="13" spans="1:17" ht="13" x14ac:dyDescent="0.25">
       <c r="A13" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="80" t="s">
+      <c r="B13" s="68" t="s">
         <v>92</v>
       </c>
-      <c r="C13" s="80"/>
-      <c r="D13" s="80"/>
-      <c r="E13" s="80"/>
-      <c r="F13" s="80"/>
-      <c r="G13" s="80"/>
-      <c r="H13" s="80"/>
-      <c r="I13" s="80"/>
-      <c r="J13" s="80"/>
-      <c r="K13" s="80"/>
-      <c r="L13" s="80"/>
-      <c r="M13" s="80"/>
-      <c r="N13" s="80"/>
-      <c r="O13" s="80"/>
-      <c r="P13" s="80"/>
-      <c r="Q13" s="81"/>
+      <c r="C13" s="68"/>
+      <c r="D13" s="68"/>
+      <c r="E13" s="68"/>
+      <c r="F13" s="68"/>
+      <c r="G13" s="68"/>
+      <c r="H13" s="68"/>
+      <c r="I13" s="68"/>
+      <c r="J13" s="68"/>
+      <c r="K13" s="68"/>
+      <c r="L13" s="68"/>
+      <c r="M13" s="68"/>
+      <c r="N13" s="68"/>
+      <c r="O13" s="68"/>
+      <c r="P13" s="68"/>
+      <c r="Q13" s="69"/>
     </row>
     <row r="14" spans="1:17" ht="13" x14ac:dyDescent="0.25">
       <c r="A14" s="35" t="s">
         <v>27</v>
       </c>
-      <c r="B14" s="82" t="s">
+      <c r="B14" s="77" t="s">
         <v>93</v>
       </c>
-      <c r="C14" s="82"/>
-      <c r="D14" s="82"/>
-      <c r="E14" s="82"/>
-      <c r="F14" s="82"/>
-      <c r="G14" s="82"/>
-      <c r="H14" s="82"/>
-      <c r="I14" s="82"/>
-      <c r="J14" s="82"/>
-      <c r="K14" s="82"/>
-      <c r="L14" s="82"/>
-      <c r="M14" s="82"/>
-      <c r="N14" s="82"/>
-      <c r="O14" s="82"/>
-      <c r="P14" s="82"/>
-      <c r="Q14" s="83"/>
+      <c r="C14" s="77"/>
+      <c r="D14" s="77"/>
+      <c r="E14" s="77"/>
+      <c r="F14" s="77"/>
+      <c r="G14" s="77"/>
+      <c r="H14" s="77"/>
+      <c r="I14" s="77"/>
+      <c r="J14" s="77"/>
+      <c r="K14" s="77"/>
+      <c r="L14" s="77"/>
+      <c r="M14" s="77"/>
+      <c r="N14" s="77"/>
+      <c r="O14" s="77"/>
+      <c r="P14" s="77"/>
+      <c r="Q14" s="78"/>
     </row>
     <row r="15" spans="1:17" ht="13" x14ac:dyDescent="0.25">
       <c r="A15" s="34" t="s">
         <v>28</v>
       </c>
-      <c r="B15" s="84" t="s">
+      <c r="B15" s="73" t="s">
         <v>94</v>
       </c>
-      <c r="C15" s="84"/>
-      <c r="D15" s="84"/>
-      <c r="E15" s="84"/>
-      <c r="F15" s="84"/>
-      <c r="G15" s="84"/>
-      <c r="H15" s="84"/>
-      <c r="I15" s="84"/>
-      <c r="J15" s="84"/>
-      <c r="K15" s="84"/>
-      <c r="L15" s="84"/>
-      <c r="M15" s="84"/>
-      <c r="N15" s="84"/>
-      <c r="O15" s="84"/>
-      <c r="P15" s="84"/>
-      <c r="Q15" s="85"/>
+      <c r="C15" s="73"/>
+      <c r="D15" s="73"/>
+      <c r="E15" s="73"/>
+      <c r="F15" s="73"/>
+      <c r="G15" s="73"/>
+      <c r="H15" s="73"/>
+      <c r="I15" s="73"/>
+      <c r="J15" s="73"/>
+      <c r="K15" s="73"/>
+      <c r="L15" s="73"/>
+      <c r="M15" s="73"/>
+      <c r="N15" s="73"/>
+      <c r="O15" s="73"/>
+      <c r="P15" s="73"/>
+      <c r="Q15" s="74"/>
     </row>
     <row r="16" spans="1:17" ht="13" x14ac:dyDescent="0.25">
       <c r="A16" s="34" t="s">
         <v>29</v>
       </c>
-      <c r="B16" s="84" t="s">
+      <c r="B16" s="73" t="s">
         <v>95</v>
       </c>
-      <c r="C16" s="84"/>
-      <c r="D16" s="84"/>
-      <c r="E16" s="84"/>
-      <c r="F16" s="84"/>
-      <c r="G16" s="84"/>
-      <c r="H16" s="84"/>
-      <c r="I16" s="84"/>
-      <c r="J16" s="84"/>
-      <c r="K16" s="84"/>
-      <c r="L16" s="84"/>
-      <c r="M16" s="84"/>
-      <c r="N16" s="84"/>
-      <c r="O16" s="84"/>
-      <c r="P16" s="84"/>
-      <c r="Q16" s="85"/>
+      <c r="C16" s="73"/>
+      <c r="D16" s="73"/>
+      <c r="E16" s="73"/>
+      <c r="F16" s="73"/>
+      <c r="G16" s="73"/>
+      <c r="H16" s="73"/>
+      <c r="I16" s="73"/>
+      <c r="J16" s="73"/>
+      <c r="K16" s="73"/>
+      <c r="L16" s="73"/>
+      <c r="M16" s="73"/>
+      <c r="N16" s="73"/>
+      <c r="O16" s="73"/>
+      <c r="P16" s="73"/>
+      <c r="Q16" s="74"/>
     </row>
     <row r="17" spans="1:17" ht="13" x14ac:dyDescent="0.25">
       <c r="A17" s="34" t="s">
         <v>30</v>
       </c>
-      <c r="B17" s="84" t="s">
+      <c r="B17" s="73" t="s">
         <v>96</v>
       </c>
-      <c r="C17" s="84"/>
-      <c r="D17" s="84"/>
-      <c r="E17" s="84"/>
-      <c r="F17" s="84"/>
-      <c r="G17" s="84"/>
-      <c r="H17" s="84"/>
-      <c r="I17" s="84"/>
-      <c r="J17" s="84"/>
-      <c r="K17" s="84"/>
-      <c r="L17" s="84"/>
-      <c r="M17" s="84"/>
-      <c r="N17" s="84"/>
-      <c r="O17" s="84"/>
-      <c r="P17" s="84"/>
-      <c r="Q17" s="85"/>
+      <c r="C17" s="73"/>
+      <c r="D17" s="73"/>
+      <c r="E17" s="73"/>
+      <c r="F17" s="73"/>
+      <c r="G17" s="73"/>
+      <c r="H17" s="73"/>
+      <c r="I17" s="73"/>
+      <c r="J17" s="73"/>
+      <c r="K17" s="73"/>
+      <c r="L17" s="73"/>
+      <c r="M17" s="73"/>
+      <c r="N17" s="73"/>
+      <c r="O17" s="73"/>
+      <c r="P17" s="73"/>
+      <c r="Q17" s="74"/>
     </row>
     <row r="18" spans="1:17" ht="13" x14ac:dyDescent="0.25">
       <c r="A18" s="34"/>
-      <c r="B18" s="78"/>
-      <c r="C18" s="78"/>
-      <c r="D18" s="78"/>
-      <c r="E18" s="78"/>
-      <c r="F18" s="78"/>
-      <c r="G18" s="78"/>
-      <c r="H18" s="78"/>
-      <c r="I18" s="78"/>
-      <c r="J18" s="78"/>
-      <c r="K18" s="78"/>
-      <c r="L18" s="78"/>
-      <c r="M18" s="78"/>
-      <c r="N18" s="78"/>
-      <c r="O18" s="78"/>
-      <c r="P18" s="78"/>
-      <c r="Q18" s="79"/>
+      <c r="B18" s="75"/>
+      <c r="C18" s="75"/>
+      <c r="D18" s="75"/>
+      <c r="E18" s="75"/>
+      <c r="F18" s="75"/>
+      <c r="G18" s="75"/>
+      <c r="H18" s="75"/>
+      <c r="I18" s="75"/>
+      <c r="J18" s="75"/>
+      <c r="K18" s="75"/>
+      <c r="L18" s="75"/>
+      <c r="M18" s="75"/>
+      <c r="N18" s="75"/>
+      <c r="O18" s="75"/>
+      <c r="P18" s="75"/>
+      <c r="Q18" s="76"/>
     </row>
     <row r="19" spans="1:17" ht="14.5" x14ac:dyDescent="0.25">
-      <c r="A19" s="68" t="s">
+      <c r="A19" s="79" t="s">
         <v>31</v>
       </c>
-      <c r="B19" s="69"/>
-      <c r="C19" s="69"/>
-      <c r="D19" s="69"/>
-      <c r="E19" s="69"/>
-      <c r="F19" s="69"/>
-      <c r="G19" s="69"/>
-      <c r="H19" s="69"/>
-      <c r="I19" s="69"/>
-      <c r="J19" s="69"/>
-      <c r="K19" s="69"/>
-      <c r="L19" s="69"/>
-      <c r="M19" s="69"/>
-      <c r="N19" s="69"/>
-      <c r="O19" s="69"/>
-      <c r="P19" s="69"/>
-      <c r="Q19" s="70"/>
+      <c r="B19" s="80"/>
+      <c r="C19" s="80"/>
+      <c r="D19" s="80"/>
+      <c r="E19" s="80"/>
+      <c r="F19" s="80"/>
+      <c r="G19" s="80"/>
+      <c r="H19" s="80"/>
+      <c r="I19" s="80"/>
+      <c r="J19" s="80"/>
+      <c r="K19" s="80"/>
+      <c r="L19" s="80"/>
+      <c r="M19" s="80"/>
+      <c r="N19" s="80"/>
+      <c r="O19" s="80"/>
+      <c r="P19" s="80"/>
+      <c r="Q19" s="81"/>
     </row>
     <row r="20" spans="1:17" ht="13" x14ac:dyDescent="0.25">
       <c r="A20" s="36">
         <v>1</v>
       </c>
-      <c r="B20" s="71" t="s">
+      <c r="B20" s="82" t="s">
         <v>32</v>
       </c>
-      <c r="C20" s="71"/>
-      <c r="D20" s="71"/>
-      <c r="E20" s="71"/>
-      <c r="F20" s="71"/>
-      <c r="G20" s="71"/>
-      <c r="H20" s="71"/>
-      <c r="I20" s="71"/>
-      <c r="J20" s="71"/>
-      <c r="K20" s="71"/>
-      <c r="L20" s="71"/>
-      <c r="M20" s="71"/>
-      <c r="N20" s="71"/>
-      <c r="O20" s="71"/>
-      <c r="P20" s="71"/>
-      <c r="Q20" s="72"/>
+      <c r="C20" s="82"/>
+      <c r="D20" s="82"/>
+      <c r="E20" s="82"/>
+      <c r="F20" s="82"/>
+      <c r="G20" s="82"/>
+      <c r="H20" s="82"/>
+      <c r="I20" s="82"/>
+      <c r="J20" s="82"/>
+      <c r="K20" s="82"/>
+      <c r="L20" s="82"/>
+      <c r="M20" s="82"/>
+      <c r="N20" s="82"/>
+      <c r="O20" s="82"/>
+      <c r="P20" s="82"/>
+      <c r="Q20" s="83"/>
     </row>
     <row r="21" spans="1:17" ht="13" x14ac:dyDescent="0.25">
       <c r="A21" s="36">
         <v>2</v>
       </c>
-      <c r="B21" s="73" t="s">
+      <c r="B21" s="84" t="s">
         <v>33</v>
       </c>
-      <c r="C21" s="74"/>
-      <c r="D21" s="74"/>
-      <c r="E21" s="74"/>
-      <c r="F21" s="74"/>
-      <c r="G21" s="74"/>
-      <c r="H21" s="74"/>
-      <c r="I21" s="74"/>
-      <c r="J21" s="74"/>
-      <c r="K21" s="74"/>
-      <c r="L21" s="74"/>
-      <c r="M21" s="74"/>
-      <c r="N21" s="74"/>
-      <c r="O21" s="74"/>
-      <c r="P21" s="74"/>
-      <c r="Q21" s="75"/>
+      <c r="C21" s="85"/>
+      <c r="D21" s="85"/>
+      <c r="E21" s="85"/>
+      <c r="F21" s="85"/>
+      <c r="G21" s="85"/>
+      <c r="H21" s="85"/>
+      <c r="I21" s="85"/>
+      <c r="J21" s="85"/>
+      <c r="K21" s="85"/>
+      <c r="L21" s="85"/>
+      <c r="M21" s="85"/>
+      <c r="N21" s="85"/>
+      <c r="O21" s="85"/>
+      <c r="P21" s="85"/>
+      <c r="Q21" s="86"/>
     </row>
     <row r="22" spans="1:17" ht="13" x14ac:dyDescent="0.25">
       <c r="A22" s="36">
         <v>3</v>
       </c>
-      <c r="B22" s="71" t="s">
+      <c r="B22" s="82" t="s">
         <v>34</v>
       </c>
-      <c r="C22" s="71"/>
-      <c r="D22" s="71"/>
-      <c r="E22" s="71"/>
-      <c r="F22" s="71"/>
-      <c r="G22" s="71"/>
-      <c r="H22" s="71"/>
-      <c r="I22" s="71"/>
-      <c r="J22" s="71"/>
-      <c r="K22" s="71"/>
-      <c r="L22" s="71"/>
-      <c r="M22" s="71"/>
-      <c r="N22" s="71"/>
-      <c r="O22" s="71"/>
-      <c r="P22" s="71"/>
-      <c r="Q22" s="72"/>
+      <c r="C22" s="82"/>
+      <c r="D22" s="82"/>
+      <c r="E22" s="82"/>
+      <c r="F22" s="82"/>
+      <c r="G22" s="82"/>
+      <c r="H22" s="82"/>
+      <c r="I22" s="82"/>
+      <c r="J22" s="82"/>
+      <c r="K22" s="82"/>
+      <c r="L22" s="82"/>
+      <c r="M22" s="82"/>
+      <c r="N22" s="82"/>
+      <c r="O22" s="82"/>
+      <c r="P22" s="82"/>
+      <c r="Q22" s="83"/>
     </row>
     <row r="23" spans="1:17" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="37">
         <v>4</v>
       </c>
-      <c r="B23" s="76" t="s">
+      <c r="B23" s="87" t="s">
         <v>35</v>
       </c>
-      <c r="C23" s="76"/>
-      <c r="D23" s="76"/>
-      <c r="E23" s="76"/>
-      <c r="F23" s="76"/>
-      <c r="G23" s="76"/>
-      <c r="H23" s="76"/>
-      <c r="I23" s="76"/>
-      <c r="J23" s="76"/>
-      <c r="K23" s="76"/>
-      <c r="L23" s="76"/>
-      <c r="M23" s="76"/>
-      <c r="N23" s="76"/>
-      <c r="O23" s="76"/>
-      <c r="P23" s="76"/>
-      <c r="Q23" s="77"/>
+      <c r="C23" s="87"/>
+      <c r="D23" s="87"/>
+      <c r="E23" s="87"/>
+      <c r="F23" s="87"/>
+      <c r="G23" s="87"/>
+      <c r="H23" s="87"/>
+      <c r="I23" s="87"/>
+      <c r="J23" s="87"/>
+      <c r="K23" s="87"/>
+      <c r="L23" s="87"/>
+      <c r="M23" s="87"/>
+      <c r="N23" s="87"/>
+      <c r="O23" s="87"/>
+      <c r="P23" s="87"/>
+      <c r="Q23" s="88"/>
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="B6:Q6"/>
-    <mergeCell ref="A1:Q1"/>
-    <mergeCell ref="B2:Q2"/>
-    <mergeCell ref="B3:Q3"/>
-    <mergeCell ref="B4:Q4"/>
-    <mergeCell ref="B5:Q5"/>
+    <mergeCell ref="A19:Q19"/>
+    <mergeCell ref="B20:Q20"/>
+    <mergeCell ref="B21:Q21"/>
+    <mergeCell ref="B22:Q22"/>
+    <mergeCell ref="B23:Q23"/>
     <mergeCell ref="B18:Q18"/>
     <mergeCell ref="B7:Q7"/>
     <mergeCell ref="B8:Q8"/>
@@ -3898,11 +3897,12 @@
     <mergeCell ref="B15:Q15"/>
     <mergeCell ref="B16:Q16"/>
     <mergeCell ref="B17:Q17"/>
-    <mergeCell ref="A19:Q19"/>
-    <mergeCell ref="B20:Q20"/>
-    <mergeCell ref="B21:Q21"/>
-    <mergeCell ref="B22:Q22"/>
-    <mergeCell ref="B23:Q23"/>
+    <mergeCell ref="B6:Q6"/>
+    <mergeCell ref="A1:Q1"/>
+    <mergeCell ref="B2:Q2"/>
+    <mergeCell ref="B3:Q3"/>
+    <mergeCell ref="B4:Q4"/>
+    <mergeCell ref="B5:Q5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="43" orientation="portrait" horizontalDpi="300" r:id="rId1"/>
@@ -3941,26 +3941,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="102" t="s">
+      <c r="A1" s="89" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="103"/>
-      <c r="C1" s="103"/>
-      <c r="D1" s="103"/>
-      <c r="E1" s="103"/>
-      <c r="F1" s="103"/>
-      <c r="G1" s="103"/>
-      <c r="H1" s="103"/>
-      <c r="I1" s="103"/>
-      <c r="J1" s="103"/>
-      <c r="K1" s="103"/>
-      <c r="L1" s="103"/>
-      <c r="M1" s="103"/>
-      <c r="N1" s="103"/>
-      <c r="O1" s="103"/>
-      <c r="P1" s="103"/>
-      <c r="Q1" s="103"/>
-      <c r="R1" s="104"/>
+      <c r="B1" s="90"/>
+      <c r="C1" s="90"/>
+      <c r="D1" s="90"/>
+      <c r="E1" s="90"/>
+      <c r="F1" s="90"/>
+      <c r="G1" s="90"/>
+      <c r="H1" s="90"/>
+      <c r="I1" s="90"/>
+      <c r="J1" s="90"/>
+      <c r="K1" s="90"/>
+      <c r="L1" s="90"/>
+      <c r="M1" s="90"/>
+      <c r="N1" s="90"/>
+      <c r="O1" s="90"/>
+      <c r="P1" s="90"/>
+      <c r="Q1" s="90"/>
+      <c r="R1" s="91"/>
     </row>
     <row r="2" spans="1:20" ht="50.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="27" t="s">
@@ -4073,26 +4073,26 @@
       </c>
     </row>
     <row r="4" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="105" t="s">
+      <c r="A4" s="92" t="s">
         <v>61</v>
       </c>
-      <c r="B4" s="106"/>
-      <c r="C4" s="106"/>
-      <c r="D4" s="106"/>
-      <c r="E4" s="106"/>
-      <c r="F4" s="106"/>
-      <c r="G4" s="106"/>
-      <c r="H4" s="106"/>
-      <c r="I4" s="106"/>
-      <c r="J4" s="106"/>
-      <c r="K4" s="106"/>
-      <c r="L4" s="106"/>
-      <c r="M4" s="106"/>
-      <c r="N4" s="106"/>
-      <c r="O4" s="106"/>
-      <c r="P4" s="106"/>
-      <c r="Q4" s="106"/>
-      <c r="R4" s="107"/>
+      <c r="B4" s="93"/>
+      <c r="C4" s="93"/>
+      <c r="D4" s="93"/>
+      <c r="E4" s="93"/>
+      <c r="F4" s="93"/>
+      <c r="G4" s="93"/>
+      <c r="H4" s="93"/>
+      <c r="I4" s="93"/>
+      <c r="J4" s="93"/>
+      <c r="K4" s="93"/>
+      <c r="L4" s="93"/>
+      <c r="M4" s="93"/>
+      <c r="N4" s="93"/>
+      <c r="O4" s="93"/>
+      <c r="P4" s="93"/>
+      <c r="Q4" s="93"/>
+      <c r="R4" s="94"/>
     </row>
     <row r="5" spans="1:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="95" t="s">
@@ -4101,22 +4101,22 @@
       <c r="B5" s="96"/>
       <c r="C5" s="97"/>
       <c r="D5" s="38"/>
-      <c r="E5" s="89" t="s">
+      <c r="E5" s="98" t="s">
         <v>63</v>
       </c>
-      <c r="F5" s="90"/>
-      <c r="G5" s="90"/>
-      <c r="H5" s="90"/>
-      <c r="I5" s="90"/>
-      <c r="J5" s="90"/>
-      <c r="K5" s="90"/>
-      <c r="L5" s="90"/>
-      <c r="M5" s="90"/>
-      <c r="N5" s="90"/>
-      <c r="O5" s="90"/>
-      <c r="P5" s="90"/>
-      <c r="Q5" s="90"/>
-      <c r="R5" s="91"/>
+      <c r="F5" s="99"/>
+      <c r="G5" s="99"/>
+      <c r="H5" s="99"/>
+      <c r="I5" s="99"/>
+      <c r="J5" s="99"/>
+      <c r="K5" s="99"/>
+      <c r="L5" s="99"/>
+      <c r="M5" s="99"/>
+      <c r="N5" s="99"/>
+      <c r="O5" s="99"/>
+      <c r="P5" s="99"/>
+      <c r="Q5" s="99"/>
+      <c r="R5" s="100"/>
       <c r="T5" s="24">
         <v>3</v>
       </c>
@@ -4139,31 +4139,31 @@
       <c r="O6" s="96"/>
       <c r="P6" s="96"/>
       <c r="Q6" s="96"/>
-      <c r="R6" s="98"/>
+      <c r="R6" s="101"/>
     </row>
     <row r="7" spans="1:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="92" t="s">
+      <c r="A7" s="102" t="s">
         <v>64</v>
       </c>
-      <c r="B7" s="93"/>
-      <c r="C7" s="94"/>
+      <c r="B7" s="103"/>
+      <c r="C7" s="104"/>
       <c r="D7" s="38"/>
-      <c r="E7" s="89" t="s">
+      <c r="E7" s="98" t="s">
         <v>63</v>
       </c>
-      <c r="F7" s="90"/>
-      <c r="G7" s="90"/>
-      <c r="H7" s="90"/>
-      <c r="I7" s="90"/>
-      <c r="J7" s="90"/>
-      <c r="K7" s="90"/>
-      <c r="L7" s="90"/>
-      <c r="M7" s="90"/>
-      <c r="N7" s="90"/>
-      <c r="O7" s="90"/>
-      <c r="P7" s="90"/>
-      <c r="Q7" s="90"/>
-      <c r="R7" s="91"/>
+      <c r="F7" s="99"/>
+      <c r="G7" s="99"/>
+      <c r="H7" s="99"/>
+      <c r="I7" s="99"/>
+      <c r="J7" s="99"/>
+      <c r="K7" s="99"/>
+      <c r="L7" s="99"/>
+      <c r="M7" s="99"/>
+      <c r="N7" s="99"/>
+      <c r="O7" s="99"/>
+      <c r="P7" s="99"/>
+      <c r="Q7" s="99"/>
+      <c r="R7" s="100"/>
     </row>
     <row r="8" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="95"/>
@@ -4183,7 +4183,7 @@
       <c r="O8" s="96"/>
       <c r="P8" s="96"/>
       <c r="Q8" s="96"/>
-      <c r="R8" s="98"/>
+      <c r="R8" s="101"/>
     </row>
     <row r="9" spans="1:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="95" t="s">
@@ -4192,22 +4192,22 @@
       <c r="B9" s="96"/>
       <c r="C9" s="97"/>
       <c r="D9" s="38"/>
-      <c r="E9" s="89" t="s">
+      <c r="E9" s="98" t="s">
         <v>63</v>
       </c>
-      <c r="F9" s="90"/>
-      <c r="G9" s="90"/>
-      <c r="H9" s="90"/>
-      <c r="I9" s="90"/>
-      <c r="J9" s="90"/>
-      <c r="K9" s="90"/>
-      <c r="L9" s="90"/>
-      <c r="M9" s="90"/>
-      <c r="N9" s="90"/>
-      <c r="O9" s="90"/>
-      <c r="P9" s="90"/>
-      <c r="Q9" s="90"/>
-      <c r="R9" s="91"/>
+      <c r="F9" s="99"/>
+      <c r="G9" s="99"/>
+      <c r="H9" s="99"/>
+      <c r="I9" s="99"/>
+      <c r="J9" s="99"/>
+      <c r="K9" s="99"/>
+      <c r="L9" s="99"/>
+      <c r="M9" s="99"/>
+      <c r="N9" s="99"/>
+      <c r="O9" s="99"/>
+      <c r="P9" s="99"/>
+      <c r="Q9" s="99"/>
+      <c r="R9" s="100"/>
     </row>
     <row r="10" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="95"/>
@@ -4227,7 +4227,7 @@
       <c r="O10" s="96"/>
       <c r="P10" s="96"/>
       <c r="Q10" s="96"/>
-      <c r="R10" s="98"/>
+      <c r="R10" s="101"/>
     </row>
     <row r="11" spans="1:20" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="95" t="s">
@@ -4236,22 +4236,22 @@
       <c r="B11" s="96"/>
       <c r="C11" s="97"/>
       <c r="D11" s="38"/>
-      <c r="E11" s="89" t="s">
+      <c r="E11" s="98" t="s">
         <v>67</v>
       </c>
-      <c r="F11" s="90"/>
-      <c r="G11" s="90"/>
-      <c r="H11" s="90"/>
-      <c r="I11" s="90"/>
-      <c r="J11" s="90"/>
-      <c r="K11" s="90"/>
-      <c r="L11" s="90"/>
-      <c r="M11" s="90"/>
-      <c r="N11" s="90"/>
-      <c r="O11" s="90"/>
-      <c r="P11" s="90"/>
-      <c r="Q11" s="90"/>
-      <c r="R11" s="91"/>
+      <c r="F11" s="99"/>
+      <c r="G11" s="99"/>
+      <c r="H11" s="99"/>
+      <c r="I11" s="99"/>
+      <c r="J11" s="99"/>
+      <c r="K11" s="99"/>
+      <c r="L11" s="99"/>
+      <c r="M11" s="99"/>
+      <c r="N11" s="99"/>
+      <c r="O11" s="99"/>
+      <c r="P11" s="99"/>
+      <c r="Q11" s="99"/>
+      <c r="R11" s="100"/>
     </row>
     <row r="12" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="95" t="s">
@@ -4273,7 +4273,7 @@
       <c r="O12" s="96"/>
       <c r="P12" s="96"/>
       <c r="Q12" s="96"/>
-      <c r="R12" s="98"/>
+      <c r="R12" s="101"/>
     </row>
     <row r="13" spans="1:20" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="25">
@@ -4285,31 +4285,26 @@
       <c r="C13" s="26" t="s">
         <v>97</v>
       </c>
-      <c r="D13" s="99" t="s">
+      <c r="D13" s="105" t="s">
         <v>70</v>
       </c>
-      <c r="E13" s="100"/>
-      <c r="F13" s="100"/>
-      <c r="G13" s="100"/>
-      <c r="H13" s="100"/>
-      <c r="I13" s="100"/>
-      <c r="J13" s="100"/>
-      <c r="K13" s="100"/>
-      <c r="L13" s="100"/>
-      <c r="M13" s="100"/>
-      <c r="N13" s="100"/>
-      <c r="O13" s="100"/>
-      <c r="P13" s="100"/>
-      <c r="Q13" s="100"/>
-      <c r="R13" s="101"/>
+      <c r="E13" s="106"/>
+      <c r="F13" s="106"/>
+      <c r="G13" s="106"/>
+      <c r="H13" s="106"/>
+      <c r="I13" s="106"/>
+      <c r="J13" s="106"/>
+      <c r="K13" s="106"/>
+      <c r="L13" s="106"/>
+      <c r="M13" s="106"/>
+      <c r="N13" s="106"/>
+      <c r="O13" s="106"/>
+      <c r="P13" s="106"/>
+      <c r="Q13" s="106"/>
+      <c r="R13" s="107"/>
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="A1:R1"/>
-    <mergeCell ref="A4:R4"/>
-    <mergeCell ref="A5:C5"/>
-    <mergeCell ref="E5:R5"/>
-    <mergeCell ref="A6:R6"/>
     <mergeCell ref="E7:R7"/>
     <mergeCell ref="A7:C7"/>
     <mergeCell ref="A11:C11"/>
@@ -4320,6 +4315,11 @@
     <mergeCell ref="A9:C9"/>
     <mergeCell ref="E9:R9"/>
     <mergeCell ref="A10:R10"/>
+    <mergeCell ref="A1:R1"/>
+    <mergeCell ref="A4:R4"/>
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="E5:R5"/>
+    <mergeCell ref="A6:R6"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup scale="28" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -4328,10 +4328,11 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<titus xmlns="http://schemas.titus.com/TitusProperties/">
-  <TitusGUID xmlns="">b32b142f-e1a3-4636-987f-842931850c11</TitusGUID>
-  <TitusMetadata xmlns="">eyJucyI6Imh0dHA6XC9cL3d3dy50aXR1cy5jb21cL25zXC9UVExUSVRVUyIsInByb3BzIjpbeyJuIjoiQ2xhc3NpZmljYXRpb24iLCJ2YWxzIjpbeyJ2YWx1ZSI6IkludGVybmFsIn1dfV19</TitusMetadata>
-</titus>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="896f6421-0ffe-4cdf-9397-f39e719ecdb4" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4576,11 +4577,10 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="896f6421-0ffe-4cdf-9397-f39e719ecdb4" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<titus xmlns="http://schemas.titus.com/TitusProperties/">
+  <TitusGUID xmlns="">b32b142f-e1a3-4636-987f-842931850c11</TitusGUID>
+  <TitusMetadata xmlns="">eyJucyI6Imh0dHA6XC9cL3d3dy50aXR1cy5jb21cL25zXC9UVExUSVRVUyIsInByb3BzIjpbeyJuIjoiQ2xhc3NpZmljYXRpb24iLCJ2YWxzIjpbeyJ2YWx1ZSI6IkludGVybmFsIn1dfV19</TitusMetadata>
+</titus>
 </file>
 
 <file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4593,10 +4593,18 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A3EF0A4F-E3E9-4C94-9786-69F046D3300A}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EC96BEBB-37FE-4C78-B1A0-F4825207DA4D}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.titus.com/TitusProperties/"/>
-    <ds:schemaRef ds:uri=""/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="896f6421-0ffe-4cdf-9397-f39e719ecdb4"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="47b22ed6-09de-4eef-8e70-1f7bccb8aa81"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -4621,18 +4629,10 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EC96BEBB-37FE-4C78-B1A0-F4825207DA4D}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A3EF0A4F-E3E9-4C94-9786-69F046D3300A}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="896f6421-0ffe-4cdf-9397-f39e719ecdb4"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="47b22ed6-09de-4eef-8e70-1f7bccb8aa81"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.titus.com/TitusProperties/"/>
+    <ds:schemaRef ds:uri=""/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>